<commit_message>
Instalacion de Unity y creacion de paneles
Se instaló unity y se crearon los paneles del juego, menu principal. creae partida y unir partida
</commit_message>
<xml_diff>
--- a/Documentación/Cronograma.xlsx
+++ b/Documentación/Cronograma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
   <si>
     <t>Involucrados</t>
   </si>
@@ -191,6 +191,24 @@
   </si>
   <si>
     <t xml:space="preserve">   Diseño de diagrama de Networking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Creación del panel del menu principal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Creación del panel crear partida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Creación del panel unirse a partida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Creación de la escena del juego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Interacción entre escenas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Creacion de prefabs Cartas y Locuras</t>
   </si>
 </sst>
 </file>
@@ -465,12 +483,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -485,7 +497,32 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -503,6 +540,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -511,28 +551,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,288 +832,288 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BE72"/>
+  <dimension ref="A2:BE78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:C26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="42" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="21"/>
-      <c r="AE2" s="21"/>
-      <c r="AF2" s="21"/>
-      <c r="AG2" s="21"/>
-      <c r="AH2" s="21"/>
-      <c r="AI2" s="21"/>
-      <c r="AJ2" s="21"/>
-      <c r="AK2" s="21"/>
-      <c r="AL2" s="21"/>
-      <c r="AM2" s="21"/>
-      <c r="AN2" s="21"/>
-      <c r="AO2" s="21"/>
-      <c r="AP2" s="21"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+      <c r="P2" s="33"/>
+      <c r="Q2" s="33"/>
+      <c r="R2" s="33"/>
+      <c r="S2" s="33"/>
+      <c r="T2" s="33"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="33"/>
+      <c r="X2" s="33"/>
+      <c r="Y2" s="33"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="33"/>
+      <c r="AB2" s="33"/>
+      <c r="AC2" s="33"/>
+      <c r="AD2" s="33"/>
+      <c r="AE2" s="33"/>
+      <c r="AF2" s="33"/>
+      <c r="AG2" s="33"/>
+      <c r="AH2" s="33"/>
+      <c r="AI2" s="33"/>
+      <c r="AJ2" s="33"/>
+      <c r="AK2" s="33"/>
+      <c r="AL2" s="33"/>
+      <c r="AM2" s="33"/>
+      <c r="AN2" s="33"/>
+      <c r="AO2" s="33"/>
+      <c r="AP2" s="33"/>
     </row>
     <row r="3" spans="1:57" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="43" t="s">
+      <c r="B3" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="44" t="s">
+      <c r="D3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="44"/>
-      <c r="L3" s="44"/>
-      <c r="M3" s="44"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="44"/>
-      <c r="P3" s="44"/>
-      <c r="Q3" s="44"/>
-      <c r="R3" s="44"/>
-      <c r="S3" s="44"/>
-      <c r="T3" s="44"/>
-      <c r="U3" s="44"/>
-      <c r="V3" s="44"/>
-      <c r="W3" s="44"/>
-      <c r="X3" s="44"/>
-      <c r="Y3" s="44"/>
-      <c r="Z3" s="44"/>
-      <c r="AA3" s="44"/>
-      <c r="AB3" s="44"/>
-      <c r="AC3" s="44"/>
-      <c r="AD3" s="44"/>
-      <c r="AE3" s="44"/>
-      <c r="AF3" s="44"/>
-      <c r="AG3" s="44"/>
-      <c r="AH3" s="44"/>
-      <c r="AI3" s="44"/>
-      <c r="AJ3" s="44"/>
-      <c r="AK3" s="44"/>
-      <c r="AL3" s="44"/>
-      <c r="AM3" s="44"/>
-      <c r="AN3" s="44"/>
-      <c r="AO3" s="44"/>
-      <c r="AP3" s="44"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="T3" s="37"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="37"/>
+      <c r="W3" s="37"/>
+      <c r="X3" s="37"/>
+      <c r="Y3" s="37"/>
+      <c r="Z3" s="37"/>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37"/>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37"/>
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37"/>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="37"/>
+      <c r="AO3" s="37"/>
+      <c r="AP3" s="37"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B4" s="43"/>
-      <c r="C4" s="46"/>
-      <c r="D4" s="45" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45" t="s">
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
-      <c r="Y4" s="45"/>
-      <c r="Z4" s="45"/>
-      <c r="AA4" s="45"/>
-      <c r="AB4" s="45"/>
-      <c r="AC4" s="45"/>
-      <c r="AD4" s="45"/>
-      <c r="AE4" s="45"/>
-      <c r="AF4" s="45"/>
-      <c r="AG4" s="45"/>
-      <c r="AH4" s="45"/>
-      <c r="AI4" s="45"/>
-      <c r="AJ4" s="45"/>
-      <c r="AK4" s="45"/>
-      <c r="AL4" s="45"/>
-      <c r="AM4" s="45"/>
-      <c r="AN4" s="45"/>
-      <c r="AO4" s="45"/>
-      <c r="AP4" s="45"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
+      <c r="AG4" s="36"/>
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="36"/>
+      <c r="AJ4" s="36"/>
+      <c r="AK4" s="36"/>
+      <c r="AL4" s="36"/>
+      <c r="AM4" s="36"/>
+      <c r="AN4" s="36"/>
+      <c r="AO4" s="36"/>
+      <c r="AP4" s="36"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B5" s="43"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="47">
+      <c r="B5" s="35"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="32">
         <v>23</v>
       </c>
-      <c r="E5" s="47">
+      <c r="E5" s="32">
         <v>24</v>
       </c>
-      <c r="F5" s="47">
+      <c r="F5" s="32">
         <v>25</v>
       </c>
-      <c r="G5" s="47">
+      <c r="G5" s="32">
         <v>26</v>
       </c>
-      <c r="H5" s="47">
+      <c r="H5" s="32">
         <v>27</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="32">
         <v>28</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J5" s="32">
         <v>29</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="32">
         <v>30</v>
       </c>
-      <c r="L5" s="47">
+      <c r="L5" s="32">
         <v>31</v>
       </c>
-      <c r="M5" s="47">
+      <c r="M5" s="32">
         <v>1</v>
       </c>
-      <c r="N5" s="47">
+      <c r="N5" s="32">
         <v>2</v>
       </c>
-      <c r="O5" s="47">
+      <c r="O5" s="32">
         <v>3</v>
       </c>
-      <c r="P5" s="47">
+      <c r="P5" s="32">
         <v>4</v>
       </c>
-      <c r="Q5" s="47">
+      <c r="Q5" s="32">
         <v>5</v>
       </c>
-      <c r="R5" s="47">
+      <c r="R5" s="32">
         <v>6</v>
       </c>
-      <c r="S5" s="47">
+      <c r="S5" s="32">
         <v>7</v>
       </c>
-      <c r="T5" s="47">
+      <c r="T5" s="32">
         <v>8</v>
       </c>
-      <c r="U5" s="47">
+      <c r="U5" s="32">
         <v>9</v>
       </c>
-      <c r="V5" s="47">
+      <c r="V5" s="32">
         <v>10</v>
       </c>
-      <c r="W5" s="47">
+      <c r="W5" s="32">
         <v>11</v>
       </c>
-      <c r="X5" s="47">
+      <c r="X5" s="32">
         <v>12</v>
       </c>
-      <c r="Y5" s="47">
+      <c r="Y5" s="32">
         <v>13</v>
       </c>
-      <c r="Z5" s="47">
+      <c r="Z5" s="32">
         <v>14</v>
       </c>
-      <c r="AA5" s="47">
+      <c r="AA5" s="32">
         <v>15</v>
       </c>
-      <c r="AB5" s="47">
+      <c r="AB5" s="32">
         <v>16</v>
       </c>
-      <c r="AC5" s="47">
+      <c r="AC5" s="32">
         <v>17</v>
       </c>
-      <c r="AD5" s="47">
+      <c r="AD5" s="32">
         <v>18</v>
       </c>
-      <c r="AE5" s="47">
+      <c r="AE5" s="32">
         <v>19</v>
       </c>
-      <c r="AF5" s="47">
+      <c r="AF5" s="32">
         <v>20</v>
       </c>
-      <c r="AG5" s="47">
+      <c r="AG5" s="32">
         <v>21</v>
       </c>
-      <c r="AH5" s="47">
+      <c r="AH5" s="32">
         <v>22</v>
       </c>
-      <c r="AI5" s="47">
+      <c r="AI5" s="32">
         <v>23</v>
       </c>
-      <c r="AJ5" s="47">
+      <c r="AJ5" s="32">
         <v>24</v>
       </c>
-      <c r="AK5" s="47">
+      <c r="AK5" s="32">
         <v>25</v>
       </c>
-      <c r="AL5" s="47">
+      <c r="AL5" s="32">
         <v>26</v>
       </c>
-      <c r="AM5" s="47">
+      <c r="AM5" s="32">
         <v>27</v>
       </c>
-      <c r="AN5" s="47">
+      <c r="AN5" s="32">
         <v>28</v>
       </c>
-      <c r="AO5" s="47">
+      <c r="AO5" s="32">
         <v>29</v>
       </c>
-      <c r="AP5" s="47">
+      <c r="AP5" s="32">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="31"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -1152,13 +1170,13 @@
       <c r="BE6" s="11"/>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="32" t="s">
+      <c r="C7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="40"/>
+      <c r="D7" s="29"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
@@ -1202,8 +1220,8 @@
       <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="33"/>
-      <c r="D8" s="40"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="29"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -1244,11 +1262,11 @@
       <c r="AP8" s="2"/>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="40"/>
+      <c r="C9" s="43"/>
+      <c r="D9" s="29"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -1289,14 +1307,14 @@
       <c r="AP9" s="2"/>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1336,15 +1354,15 @@
       <c r="AP10" s="2"/>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="23" t="s">
         <v>33</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
       <c r="F11" s="1"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -1384,15 +1402,15 @@
       <c r="AP11" s="2"/>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="41" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="41"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
       <c r="G12" s="13"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -1431,13 +1449,13 @@
       <c r="AP12" s="2"/>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="33"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="41"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
       <c r="G13" s="13"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
@@ -1476,13 +1494,13 @@
       <c r="AP13" s="2"/>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="33"/>
+      <c r="C14" s="42"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="41"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
       <c r="G14" s="13"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
@@ -1521,13 +1539,13 @@
       <c r="AP14" s="2"/>
     </row>
     <row r="15" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C15" s="33"/>
+      <c r="C15" s="42"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="41"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
       <c r="G15" s="13"/>
       <c r="H15" s="10"/>
       <c r="I15" s="10"/>
@@ -1566,13 +1584,13 @@
       <c r="AP15" s="2"/>
     </row>
     <row r="16" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="34"/>
+      <c r="C16" s="43"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="41"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
       <c r="G16" s="13"/>
       <c r="H16" s="10"/>
       <c r="I16" s="10"/>
@@ -1611,16 +1629,16 @@
       <c r="AP16" s="2"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="47" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="40"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="29"/>
       <c r="H17" s="1"/>
       <c r="I17" s="10"/>
       <c r="J17" s="7"/>
@@ -1658,14 +1676,14 @@
       <c r="AP17" s="2"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
+      <c r="C18" s="48"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="40"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="29"/>
       <c r="H18" s="1"/>
       <c r="I18" s="10"/>
       <c r="J18" s="7"/>
@@ -1703,14 +1721,14 @@
       <c r="AP18" s="2"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="39"/>
+      <c r="C19" s="49"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="40"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="29"/>
       <c r="H19" s="1"/>
       <c r="I19" s="10"/>
       <c r="J19" s="7"/>
@@ -1748,18 +1766,18 @@
       <c r="AP19" s="2"/>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="44" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
       <c r="J20" s="7"/>
       <c r="K20" s="1"/>
       <c r="L20" s="2"/>
@@ -1795,16 +1813,16 @@
       <c r="AP20" s="2"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="48"/>
+      <c r="C21" s="46"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
       <c r="J21" s="7"/>
       <c r="K21" s="1"/>
       <c r="L21" s="2"/>
@@ -1840,17 +1858,17 @@
       <c r="AP21" s="2"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="23"/>
       <c r="B22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="36"/>
+      <c r="C22" s="45"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
       <c r="J22" s="7"/>
       <c r="K22" s="1"/>
       <c r="L22" s="2"/>
@@ -1886,10 +1904,10 @@
       <c r="AP22" s="2"/>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="47" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="2"/>
@@ -1899,8 +1917,8 @@
       <c r="H23" s="2"/>
       <c r="I23" s="10"/>
       <c r="J23" s="7"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
       <c r="M23" s="1"/>
       <c r="N23" s="10"/>
       <c r="O23" s="2"/>
@@ -1936,7 +1954,7 @@
       <c r="B24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="38"/>
+      <c r="C24" s="48"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1944,8 +1962,8 @@
       <c r="H24" s="2"/>
       <c r="I24" s="10"/>
       <c r="J24" s="7"/>
-      <c r="K24" s="40"/>
-      <c r="L24" s="40"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
       <c r="M24" s="1"/>
       <c r="N24" s="10"/>
       <c r="O24" s="2"/>
@@ -1981,7 +1999,7 @@
       <c r="B25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="39"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -1989,8 +2007,8 @@
       <c r="H25" s="2"/>
       <c r="I25" s="10"/>
       <c r="J25" s="7"/>
-      <c r="K25" s="40"/>
-      <c r="L25" s="40"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
       <c r="M25" s="1"/>
       <c r="N25" s="10"/>
       <c r="O25" s="2"/>
@@ -2023,10 +2041,10 @@
       <c r="AP25" s="2"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B26" s="49" t="s">
+      <c r="B26" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="49"/>
+      <c r="C26" s="40"/>
       <c r="D26" s="10"/>
       <c r="E26" s="10"/>
       <c r="F26" s="10"/>
@@ -2076,7 +2094,7 @@
       <c r="AX26" s="11"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="22" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="1"/>
@@ -2089,8 +2107,8 @@
       <c r="J27" s="7"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="40"/>
-      <c r="N27" s="40"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
       <c r="Q27" s="7"/>
@@ -2122,7 +2140,7 @@
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>14</v>
+        <v>41</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
@@ -2134,14 +2152,14 @@
       <c r="J28" s="7"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
       <c r="O28" s="1"/>
-      <c r="P28" s="10"/>
+      <c r="P28" s="1"/>
       <c r="Q28" s="7"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
+      <c r="R28" s="2"/>
+      <c r="S28" s="2"/>
+      <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
       <c r="W28" s="10"/>
@@ -2167,7 +2185,7 @@
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="2"/>
@@ -2179,17 +2197,17 @@
       <c r="J29" s="7"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="40"/>
-      <c r="P29" s="40"/>
-      <c r="Q29" s="19"/>
-      <c r="R29" s="40"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="2"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
+      <c r="U29" s="2"/>
+      <c r="V29" s="2"/>
+      <c r="W29" s="10"/>
       <c r="X29" s="7"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
@@ -2212,7 +2230,7 @@
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="2"/>
@@ -2224,27 +2242,27 @@
       <c r="J30" s="7"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="10"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
       <c r="Q30" s="7"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="40"/>
-      <c r="T30" s="40"/>
-      <c r="U30" s="40"/>
-      <c r="V30" s="40"/>
-      <c r="W30" s="40"/>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+      <c r="U30" s="2"/>
+      <c r="V30" s="2"/>
+      <c r="W30" s="10"/>
       <c r="X30" s="7"/>
-      <c r="Y30" s="1"/>
-      <c r="Z30" s="1"/>
-      <c r="AA30" s="1"/>
-      <c r="AB30" s="1"/>
-      <c r="AC30" s="1"/>
+      <c r="Y30" s="2"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="2"/>
+      <c r="AB30" s="2"/>
+      <c r="AC30" s="2"/>
       <c r="AD30" s="10"/>
       <c r="AE30" s="7"/>
-      <c r="AF30" s="10"/>
-      <c r="AG30" s="10"/>
+      <c r="AF30" s="2"/>
+      <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
       <c r="AJ30" s="2"/>
@@ -2256,8 +2274,11 @@
       <c r="AP30" s="2"/>
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
       <c r="B31" s="4" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="2"/>
@@ -2269,27 +2290,27 @@
       <c r="J31" s="7"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" s="2"/>
-      <c r="P31" s="10"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
       <c r="Q31" s="7"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="10"/>
+      <c r="S31" s="2"/>
       <c r="T31" s="2"/>
-      <c r="U31" s="40"/>
-      <c r="V31" s="40"/>
-      <c r="W31" s="40"/>
+      <c r="U31" s="2"/>
+      <c r="V31" s="2"/>
+      <c r="W31" s="10"/>
       <c r="X31" s="7"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
-      <c r="AD31" s="1"/>
+      <c r="AD31" s="10"/>
       <c r="AE31" s="7"/>
-      <c r="AF31" s="10"/>
-      <c r="AG31" s="10"/>
+      <c r="AF31" s="2"/>
+      <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
       <c r="AJ31" s="2"/>
@@ -2301,8 +2322,8 @@
       <c r="AP31" s="2"/>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>15</v>
+      <c r="B32" s="22" t="s">
+        <v>14</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="2"/>
@@ -2314,31 +2335,31 @@
       <c r="J32" s="7"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="1"/>
       <c r="P32" s="10"/>
       <c r="Q32" s="7"/>
-      <c r="R32" s="2"/>
-      <c r="S32" s="2"/>
-      <c r="T32" s="2"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
       <c r="W32" s="10"/>
       <c r="X32" s="7"/>
-      <c r="Y32" s="40"/>
-      <c r="Z32" s="40"/>
-      <c r="AA32" s="40"/>
-      <c r="AB32" s="40"/>
-      <c r="AC32" s="40"/>
+      <c r="Y32" s="2"/>
+      <c r="Z32" s="2"/>
+      <c r="AA32" s="2"/>
+      <c r="AB32" s="2"/>
+      <c r="AC32" s="2"/>
       <c r="AD32" s="10"/>
       <c r="AE32" s="7"/>
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
-      <c r="AH32" s="1"/>
-      <c r="AI32" s="1"/>
-      <c r="AJ32" s="1"/>
-      <c r="AK32" s="1"/>
+      <c r="AH32" s="2"/>
+      <c r="AI32" s="2"/>
+      <c r="AJ32" s="2"/>
+      <c r="AK32" s="10"/>
       <c r="AL32" s="10"/>
       <c r="AM32" s="2"/>
       <c r="AN32" s="2"/>
@@ -2346,54 +2367,53 @@
       <c r="AP32" s="2"/>
     </row>
     <row r="33" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B33" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="31"/>
+      <c r="B33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="1"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-      <c r="H33" s="10"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
+      <c r="H33" s="2"/>
       <c r="I33" s="10"/>
       <c r="J33" s="7"/>
-      <c r="K33" s="10"/>
-      <c r="L33" s="10"/>
-      <c r="M33" s="10"/>
-      <c r="N33" s="10"/>
-      <c r="O33" s="10"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="1"/>
       <c r="P33" s="10"/>
       <c r="Q33" s="7"/>
-      <c r="R33" s="10"/>
-      <c r="S33" s="10"/>
-      <c r="T33" s="10"/>
-      <c r="U33" s="10"/>
-      <c r="V33" s="10"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="2"/>
+      <c r="V33" s="2"/>
       <c r="W33" s="10"/>
       <c r="X33" s="7"/>
-      <c r="Y33" s="10"/>
-      <c r="Z33" s="10"/>
-      <c r="AA33" s="10"/>
-      <c r="AB33" s="10"/>
-      <c r="AC33" s="10"/>
-      <c r="AD33" s="16"/>
-      <c r="AE33" s="16"/>
-      <c r="AF33" s="16"/>
-      <c r="AG33" s="16"/>
-      <c r="AH33" s="18"/>
-      <c r="AI33" s="18"/>
-      <c r="AJ33" s="18"/>
-      <c r="AK33" s="13"/>
+      <c r="Y33" s="2"/>
+      <c r="Z33" s="2"/>
+      <c r="AA33" s="2"/>
+      <c r="AB33" s="2"/>
+      <c r="AC33" s="2"/>
+      <c r="AD33" s="10"/>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="2"/>
+      <c r="AG33" s="2"/>
+      <c r="AH33" s="2"/>
+      <c r="AI33" s="2"/>
+      <c r="AJ33" s="2"/>
+      <c r="AK33" s="10"/>
       <c r="AL33" s="10"/>
-      <c r="AM33" s="10"/>
-      <c r="AN33" s="10"/>
-      <c r="AO33" s="10"/>
-      <c r="AP33" s="10"/>
-      <c r="AQ33" s="11"/>
+      <c r="AM33" s="2"/>
+      <c r="AN33" s="2"/>
+      <c r="AO33" s="2"/>
+      <c r="AP33" s="2"/>
     </row>
     <row r="34" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B34" s="4" t="s">
-        <v>16</v>
+      <c r="B34" s="22" t="s">
+        <v>24</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="2"/>
@@ -2407,38 +2427,38 @@
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="7"/>
-      <c r="R34" s="2"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="29"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
-      <c r="U34" s="2"/>
-      <c r="V34" s="2"/>
-      <c r="W34" s="10"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
       <c r="X34" s="7"/>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
-      <c r="AD34" s="40"/>
-      <c r="AE34" s="5"/>
-      <c r="AF34" s="40"/>
-      <c r="AG34" s="40"/>
+      <c r="AD34" s="10"/>
+      <c r="AE34" s="7"/>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
       <c r="AJ34" s="2"/>
-      <c r="AK34" s="1"/>
+      <c r="AK34" s="10"/>
       <c r="AL34" s="10"/>
-      <c r="AM34" s="10"/>
-      <c r="AN34" s="10"/>
-      <c r="AO34" s="10"/>
+      <c r="AM34" s="2"/>
+      <c r="AN34" s="2"/>
+      <c r="AO34" s="2"/>
       <c r="AP34" s="2"/>
     </row>
     <row r="35" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>17</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -2452,15 +2472,15 @@
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="7"/>
-      <c r="R35" s="2"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="29"/>
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
-      <c r="U35" s="2"/>
-      <c r="V35" s="2"/>
-      <c r="W35" s="10"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
       <c r="X35" s="7"/>
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
@@ -2470,20 +2490,20 @@
       <c r="AD35" s="10"/>
       <c r="AE35" s="7"/>
       <c r="AF35" s="2"/>
-      <c r="AG35" s="1"/>
-      <c r="AH35" s="40"/>
-      <c r="AI35" s="40"/>
+      <c r="AG35" s="2"/>
+      <c r="AH35" s="2"/>
+      <c r="AI35" s="2"/>
       <c r="AJ35" s="2"/>
       <c r="AK35" s="10"/>
       <c r="AL35" s="10"/>
-      <c r="AM35" s="10"/>
-      <c r="AN35" s="10"/>
-      <c r="AO35" s="10"/>
+      <c r="AM35" s="2"/>
+      <c r="AN35" s="2"/>
+      <c r="AO35" s="2"/>
       <c r="AP35" s="2"/>
     </row>
     <row r="36" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
-        <v>5</v>
+      <c r="B36" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -2501,283 +2521,554 @@
       <c r="P36" s="10"/>
       <c r="Q36" s="7"/>
       <c r="R36" s="2"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="2"/>
-      <c r="U36" s="2"/>
-      <c r="V36" s="2"/>
-      <c r="W36" s="10"/>
+      <c r="S36" s="29"/>
+      <c r="T36" s="29"/>
+      <c r="U36" s="29"/>
+      <c r="V36" s="29"/>
+      <c r="W36" s="29"/>
       <c r="X36" s="7"/>
-      <c r="Y36" s="2"/>
-      <c r="Z36" s="2"/>
-      <c r="AA36" s="2"/>
-      <c r="AB36" s="2"/>
-      <c r="AC36" s="2"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
+      <c r="AB36" s="1"/>
+      <c r="AC36" s="1"/>
       <c r="AD36" s="10"/>
       <c r="AE36" s="7"/>
-      <c r="AF36" s="2"/>
-      <c r="AG36" s="2"/>
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="10"/>
       <c r="AH36" s="2"/>
-      <c r="AI36" s="1"/>
-      <c r="AJ36" s="40"/>
-      <c r="AK36" s="1"/>
+      <c r="AI36" s="2"/>
+      <c r="AJ36" s="2"/>
+      <c r="AK36" s="10"/>
       <c r="AL36" s="10"/>
-      <c r="AM36" s="10"/>
-      <c r="AN36" s="10"/>
-      <c r="AO36" s="12"/>
+      <c r="AM36" s="2"/>
+      <c r="AN36" s="2"/>
+      <c r="AO36" s="2"/>
       <c r="AP36" s="2"/>
     </row>
     <row r="37" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="20"/>
-      <c r="Y37" s="20"/>
-      <c r="Z37" s="20"/>
-      <c r="AA37" s="20"/>
-      <c r="AB37" s="20"/>
-      <c r="AC37" s="20"/>
-      <c r="AD37" s="20"/>
-      <c r="AE37" s="20"/>
-      <c r="AF37" s="20"/>
-      <c r="AG37" s="20"/>
-      <c r="AH37" s="20"/>
-      <c r="AI37" s="20"/>
-      <c r="AJ37" s="20"/>
-      <c r="AK37" s="20"/>
-      <c r="AL37" s="20"/>
-      <c r="AM37" s="20"/>
-      <c r="AN37" s="20"/>
-      <c r="AO37" s="20"/>
-      <c r="AP37" s="20"/>
+      <c r="B37" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="1"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+      <c r="O37" s="2"/>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="2"/>
+      <c r="S37" s="10"/>
+      <c r="T37" s="2"/>
+      <c r="U37" s="29"/>
+      <c r="V37" s="29"/>
+      <c r="W37" s="29"/>
+      <c r="X37" s="7"/>
+      <c r="Y37" s="2"/>
+      <c r="Z37" s="2"/>
+      <c r="AA37" s="2"/>
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="1"/>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="10"/>
+      <c r="AH37" s="2"/>
+      <c r="AI37" s="2"/>
+      <c r="AJ37" s="2"/>
+      <c r="AK37" s="10"/>
+      <c r="AL37" s="10"/>
+      <c r="AM37" s="2"/>
+      <c r="AN37" s="2"/>
+      <c r="AO37" s="2"/>
+      <c r="AP37" s="2"/>
     </row>
     <row r="38" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="20"/>
-      <c r="W38" s="20"/>
-      <c r="X38" s="20"/>
-      <c r="Y38" s="20"/>
-      <c r="Z38" s="20"/>
-      <c r="AA38" s="20"/>
-      <c r="AB38" s="20"/>
-      <c r="AC38" s="20"/>
-      <c r="AD38" s="20"/>
-      <c r="AE38" s="20"/>
-      <c r="AF38" s="20"/>
-      <c r="AG38" s="20"/>
-      <c r="AH38" s="20"/>
-      <c r="AI38" s="20"/>
-      <c r="AJ38" s="20"/>
-      <c r="AK38" s="20"/>
-      <c r="AL38" s="20"/>
-      <c r="AM38" s="20"/>
-      <c r="AN38" s="20"/>
-      <c r="AO38" s="20"/>
-      <c r="AP38" s="20"/>
+      <c r="B38" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="10"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="2"/>
+      <c r="S38" s="2"/>
+      <c r="T38" s="2"/>
+      <c r="U38" s="2"/>
+      <c r="V38" s="2"/>
+      <c r="W38" s="10"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="29"/>
+      <c r="Z38" s="29"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="29"/>
+      <c r="AC38" s="29"/>
+      <c r="AD38" s="10"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="2"/>
+      <c r="AG38" s="2"/>
+      <c r="AH38" s="1"/>
+      <c r="AI38" s="1"/>
+      <c r="AJ38" s="1"/>
+      <c r="AK38" s="1"/>
+      <c r="AL38" s="10"/>
+      <c r="AM38" s="2"/>
+      <c r="AN38" s="2"/>
+      <c r="AO38" s="2"/>
+      <c r="AP38" s="2"/>
     </row>
     <row r="39" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="20"/>
-      <c r="T39" s="20"/>
-      <c r="U39" s="20"/>
-      <c r="V39" s="20"/>
-      <c r="W39" s="20"/>
-      <c r="X39" s="20"/>
-      <c r="Y39" s="20"/>
-      <c r="Z39" s="20"/>
-      <c r="AA39" s="20"/>
-      <c r="AB39" s="20"/>
-      <c r="AC39" s="20"/>
-      <c r="AD39" s="20"/>
-      <c r="AE39" s="20"/>
-      <c r="AF39" s="20"/>
-      <c r="AG39" s="20"/>
-      <c r="AH39" s="20"/>
-      <c r="AI39" s="20"/>
-      <c r="AJ39" s="20"/>
-      <c r="AK39" s="20"/>
-      <c r="AL39" s="20"/>
-      <c r="AM39" s="20"/>
-      <c r="AN39" s="20"/>
-      <c r="AO39" s="20"/>
-      <c r="AP39" s="20"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
+      <c r="B39" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="39"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+      <c r="O39" s="10"/>
+      <c r="P39" s="10"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="10"/>
+      <c r="S39" s="10"/>
+      <c r="T39" s="10"/>
+      <c r="U39" s="10"/>
+      <c r="V39" s="10"/>
+      <c r="W39" s="10"/>
+      <c r="X39" s="7"/>
+      <c r="Y39" s="10"/>
+      <c r="Z39" s="10"/>
+      <c r="AA39" s="10"/>
+      <c r="AB39" s="10"/>
+      <c r="AC39" s="10"/>
+      <c r="AD39" s="16"/>
+      <c r="AE39" s="16"/>
+      <c r="AF39" s="16"/>
+      <c r="AG39" s="16"/>
+      <c r="AH39" s="18"/>
+      <c r="AI39" s="18"/>
+      <c r="AJ39" s="18"/>
+      <c r="AK39" s="13"/>
+      <c r="AL39" s="10"/>
+      <c r="AM39" s="10"/>
+      <c r="AN39" s="10"/>
+      <c r="AO39" s="10"/>
+      <c r="AP39" s="10"/>
+      <c r="AQ39" s="11"/>
+    </row>
+    <row r="40" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B40" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2"/>
+      <c r="I40" s="10"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+      <c r="O40" s="2"/>
+      <c r="P40" s="10"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="2"/>
+      <c r="S40" s="2"/>
+      <c r="T40" s="2"/>
+      <c r="U40" s="2"/>
+      <c r="V40" s="2"/>
+      <c r="W40" s="10"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="2"/>
+      <c r="Z40" s="2"/>
+      <c r="AA40" s="2"/>
+      <c r="AB40" s="2"/>
+      <c r="AC40" s="2"/>
+      <c r="AD40" s="29"/>
+      <c r="AE40" s="5"/>
+      <c r="AF40" s="29"/>
+      <c r="AG40" s="29"/>
+      <c r="AH40" s="2"/>
+      <c r="AI40" s="2"/>
+      <c r="AJ40" s="2"/>
+      <c r="AK40" s="1"/>
+      <c r="AL40" s="10"/>
+      <c r="AM40" s="10"/>
+      <c r="AN40" s="10"/>
+      <c r="AO40" s="10"/>
+      <c r="AP40" s="2"/>
+    </row>
+    <row r="41" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B41" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="10"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+      <c r="O41" s="2"/>
+      <c r="P41" s="10"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="2"/>
+      <c r="S41" s="2"/>
+      <c r="T41" s="2"/>
+      <c r="U41" s="2"/>
+      <c r="V41" s="2"/>
+      <c r="W41" s="10"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="2"/>
+      <c r="Z41" s="2"/>
+      <c r="AA41" s="2"/>
+      <c r="AB41" s="2"/>
+      <c r="AC41" s="2"/>
+      <c r="AD41" s="10"/>
+      <c r="AE41" s="7"/>
+      <c r="AF41" s="2"/>
+      <c r="AG41" s="1"/>
+      <c r="AH41" s="29"/>
+      <c r="AI41" s="29"/>
+      <c r="AJ41" s="2"/>
+      <c r="AK41" s="10"/>
+      <c r="AL41" s="10"/>
+      <c r="AM41" s="10"/>
+      <c r="AN41" s="10"/>
+      <c r="AO41" s="10"/>
+      <c r="AP41" s="2"/>
+    </row>
+    <row r="42" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B42" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" s="1"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
+      <c r="O42" s="2"/>
+      <c r="P42" s="10"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="2"/>
+      <c r="S42" s="2"/>
+      <c r="T42" s="2"/>
+      <c r="U42" s="2"/>
+      <c r="V42" s="2"/>
+      <c r="W42" s="10"/>
+      <c r="X42" s="7"/>
+      <c r="Y42" s="2"/>
+      <c r="Z42" s="2"/>
+      <c r="AA42" s="2"/>
+      <c r="AB42" s="2"/>
+      <c r="AC42" s="2"/>
+      <c r="AD42" s="10"/>
+      <c r="AE42" s="7"/>
+      <c r="AF42" s="2"/>
+      <c r="AG42" s="2"/>
+      <c r="AH42" s="2"/>
+      <c r="AI42" s="1"/>
+      <c r="AJ42" s="29"/>
+      <c r="AK42" s="1"/>
+      <c r="AL42" s="10"/>
+      <c r="AM42" s="10"/>
+      <c r="AN42" s="10"/>
+      <c r="AO42" s="12"/>
+      <c r="AP42" s="2"/>
+    </row>
+    <row r="43" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+      <c r="I43" s="20"/>
+      <c r="J43" s="20"/>
+      <c r="K43" s="20"/>
+      <c r="L43" s="20"/>
+      <c r="M43" s="20"/>
+      <c r="N43" s="20"/>
+      <c r="O43" s="20"/>
+      <c r="P43" s="20"/>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="20"/>
+      <c r="S43" s="20"/>
+      <c r="T43" s="20"/>
+      <c r="U43" s="20"/>
+      <c r="V43" s="20"/>
+      <c r="W43" s="20"/>
+      <c r="X43" s="20"/>
+      <c r="Y43" s="20"/>
+      <c r="Z43" s="20"/>
+      <c r="AA43" s="20"/>
+      <c r="AB43" s="20"/>
+      <c r="AC43" s="20"/>
+      <c r="AD43" s="20"/>
+      <c r="AE43" s="20"/>
+      <c r="AF43" s="20"/>
+      <c r="AG43" s="20"/>
+      <c r="AH43" s="20"/>
+      <c r="AI43" s="20"/>
+      <c r="AJ43" s="20"/>
+      <c r="AK43" s="20"/>
+      <c r="AL43" s="20"/>
+      <c r="AM43" s="20"/>
+      <c r="AN43" s="20"/>
+      <c r="AO43" s="20"/>
+      <c r="AP43" s="20"/>
+    </row>
+    <row r="44" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
+      <c r="J44" s="20"/>
+      <c r="K44" s="20"/>
+      <c r="L44" s="20"/>
+      <c r="M44" s="20"/>
+      <c r="N44" s="20"/>
+      <c r="O44" s="20"/>
+      <c r="P44" s="20"/>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="20"/>
+      <c r="S44" s="20"/>
+      <c r="T44" s="20"/>
+      <c r="U44" s="20"/>
+      <c r="V44" s="20"/>
+      <c r="W44" s="20"/>
+      <c r="X44" s="20"/>
+      <c r="Y44" s="20"/>
+      <c r="Z44" s="20"/>
+      <c r="AA44" s="20"/>
+      <c r="AB44" s="20"/>
+      <c r="AC44" s="20"/>
+      <c r="AD44" s="20"/>
+      <c r="AE44" s="20"/>
+      <c r="AF44" s="20"/>
+      <c r="AG44" s="20"/>
+      <c r="AH44" s="20"/>
+      <c r="AI44" s="20"/>
+      <c r="AJ44" s="20"/>
+      <c r="AK44" s="20"/>
+      <c r="AL44" s="20"/>
+      <c r="AM44" s="20"/>
+      <c r="AN44" s="20"/>
+      <c r="AO44" s="20"/>
+      <c r="AP44" s="20"/>
+    </row>
+    <row r="45" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
+      <c r="L45" s="20"/>
+      <c r="M45" s="20"/>
+      <c r="N45" s="20"/>
+      <c r="O45" s="20"/>
+      <c r="P45" s="20"/>
+      <c r="Q45" s="20"/>
+      <c r="R45" s="20"/>
+      <c r="S45" s="20"/>
+      <c r="T45" s="20"/>
+      <c r="U45" s="20"/>
+      <c r="V45" s="20"/>
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+      <c r="Y45" s="20"/>
+      <c r="Z45" s="20"/>
+      <c r="AA45" s="20"/>
+      <c r="AB45" s="20"/>
+      <c r="AC45" s="20"/>
+      <c r="AD45" s="20"/>
+      <c r="AE45" s="20"/>
+      <c r="AF45" s="20"/>
+      <c r="AG45" s="20"/>
+      <c r="AH45" s="20"/>
+      <c r="AI45" s="20"/>
+      <c r="AJ45" s="20"/>
+      <c r="AK45" s="20"/>
+      <c r="AL45" s="20"/>
+      <c r="AM45" s="20"/>
+      <c r="AN45" s="20"/>
+      <c r="AO45" s="20"/>
+      <c r="AP45" s="20"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B51" s="26"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="22"/>
-      <c r="B52" s="26"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="22"/>
-      <c r="B53" s="26"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="15" t="s">
+      <c r="B57" s="24"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="34"/>
+      <c r="B58" s="24"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="34"/>
+      <c r="B59" s="24"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B54" s="27"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B55" s="28"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B56" s="27"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B57" s="28"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B58" s="29"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B59" s="28"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B60" s="29"/>
+      <c r="B60" s="25"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B61" s="28"/>
+      <c r="B61" s="26"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B62" s="27"/>
+      <c r="B62" s="25"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B63" s="26"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B63" s="29"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
+      <c r="B64" s="27"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B64" s="28"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B65" s="27"/>
+      <c r="B65" s="26"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B66" s="29"/>
+      <c r="B66" s="27"/>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B67" s="29"/>
+      <c r="A67" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B67" s="26"/>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="27"/>
+      <c r="B68" s="25"/>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B69" s="29"/>
+      <c r="B69" s="27"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="30"/>
+      <c r="A70" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="26"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="30"/>
+      <c r="A71" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B71" s="25"/>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="30"/>
+      <c r="A72" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B72" s="27"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B73" s="27"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B74" s="25"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B75" s="27"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="28"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="28"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="A2:AP2"/>
-    <mergeCell ref="A51:A53"/>
+    <mergeCell ref="A57:A59"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="M4:AP4"/>
     <mergeCell ref="D4:L4"/>
@@ -2785,7 +3076,7 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B39:C39"/>
     <mergeCell ref="C7:C9"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C12:C16"/>

</xml_diff>

<commit_message>
Creacion de prefabs cartas y paneles del menu
Se crearon los prefeabs de la carta, el panel de el menu principal,crear y unirse a partida
</commit_message>
<xml_diff>
--- a/Documentación/Cronograma.xlsx
+++ b/Documentación/Cronograma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t>Involucrados</t>
   </si>
@@ -459,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -526,31 +526,64 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -834,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:BE78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34:C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1632,7 +1665,7 @@
       <c r="B17" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="47" t="s">
+      <c r="C17" s="46" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="2"/>
@@ -1679,7 +1712,7 @@
       <c r="B18" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="48"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="31"/>
@@ -1724,7 +1757,7 @@
       <c r="B19" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="49"/>
+      <c r="C19" s="48"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="31"/>
@@ -1816,7 +1849,7 @@
       <c r="B21" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="46"/>
+      <c r="C21" s="49"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
@@ -1907,7 +1940,7 @@
       <c r="B23" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="47" t="s">
+      <c r="C23" s="46" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="2"/>
@@ -1954,7 +1987,7 @@
       <c r="B24" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="48"/>
+      <c r="C24" s="47"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
@@ -1999,7 +2032,7 @@
       <c r="B25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="49"/>
+      <c r="C25" s="48"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -2097,7 +2130,9 @@
       <c r="B27" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="1"/>
+      <c r="C27" s="50" t="s">
+        <v>19</v>
+      </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
@@ -2142,7 +2177,7 @@
       <c r="B28" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="1"/>
+      <c r="C28" s="51"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
@@ -2187,7 +2222,7 @@
       <c r="B29" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="1"/>
+      <c r="C29" s="51"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
@@ -2232,7 +2267,7 @@
       <c r="B30" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C30" s="1"/>
+      <c r="C30" s="51"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
@@ -2280,7 +2315,7 @@
       <c r="B31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="1"/>
+      <c r="C31" s="52"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -2325,7 +2360,9 @@
       <c r="B32" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="1"/>
+      <c r="C32" s="53" t="s">
+        <v>10</v>
+      </c>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -2370,7 +2407,7 @@
       <c r="B33" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C33" s="1"/>
+      <c r="C33" s="54"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -2415,7 +2452,9 @@
       <c r="B34" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="1"/>
+      <c r="C34" s="55" t="s">
+        <v>11</v>
+      </c>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -2460,7 +2499,7 @@
       <c r="B35" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="1"/>
+      <c r="C35" s="56"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -2505,7 +2544,9 @@
       <c r="B36" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="1"/>
+      <c r="C36" s="57" t="s">
+        <v>19</v>
+      </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -2550,7 +2591,9 @@
       <c r="B37" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="1"/>
+      <c r="C37" s="58" t="s">
+        <v>10</v>
+      </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -2595,7 +2638,9 @@
       <c r="B38" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="1"/>
+      <c r="C38" s="59" t="s">
+        <v>11</v>
+      </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -2686,7 +2731,9 @@
       <c r="B40" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C40" s="1"/>
+      <c r="C40" s="59" t="s">
+        <v>11</v>
+      </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -2731,7 +2778,9 @@
       <c r="B41" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="1"/>
+      <c r="C41" s="60" t="s">
+        <v>10</v>
+      </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -2776,7 +2825,9 @@
       <c r="B42" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="1"/>
+      <c r="C42" s="59" t="s">
+        <v>11</v>
+      </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
@@ -2958,15 +3009,9 @@
       <c r="B59" s="24"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
-        <v>10</v>
-      </c>
       <c r="B60" s="25"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>19</v>
-      </c>
       <c r="B61" s="26"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -3066,7 +3111,10 @@
       <c r="B78" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="19">
+    <mergeCell ref="C27:C31"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="C34:C35"/>
     <mergeCell ref="A2:AP2"/>
     <mergeCell ref="A57:A59"/>
     <mergeCell ref="B3:B5"/>

</xml_diff>

<commit_message>
Creación de prefab panelInfoCartas, mejora prefab Locura
Se creó el prefab de el panel que muestra la información de las cartas, y el prefab de las fichas de locuras
</commit_message>
<xml_diff>
--- a/Documentación/Cronograma.xlsx
+++ b/Documentación/Cronograma.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="51">
   <si>
     <t>Involucrados</t>
   </si>
@@ -116,30 +116,10 @@
     <t xml:space="preserve">    Diseño del Tablero de juego </t>
   </si>
   <si>
-    <t>Obtencion de componentes</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Escaneo de cartas</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">   </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">  Edicion y mejora de imagenes</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Elaboracion de casos de uso</t>
   </si>
   <si>
     <r>
@@ -184,18 +164,12 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">    Interacciones y metodos de entidades</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Conceptos del Sistema de Red</t>
   </si>
   <si>
     <t xml:space="preserve">   Diseño de diagrama de Networking</t>
   </si>
   <si>
-    <t xml:space="preserve">     Creación del panel del menu principal</t>
-  </si>
-  <si>
     <t xml:space="preserve">     Creación del panel crear partida</t>
   </si>
   <si>
@@ -208,14 +182,41 @@
     <t xml:space="preserve">    Interacción entre escenas</t>
   </si>
   <si>
-    <t xml:space="preserve">    Creacion de prefabs Cartas y Locuras</t>
+    <t xml:space="preserve">   Creación del cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Creación del servidor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Creación de instrucciones del juego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Elaboración de la caja de entrega</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Edición y mejora de imágenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Elaboración de casos de uso</t>
+  </si>
+  <si>
+    <t>Obtención de componentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Interacciones y métodos de entidades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Creación del panel del menú principal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Creación de prefabs Cartas y Locuras</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,19 +303,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="16">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -349,12 +350,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,29 +454,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -490,101 +481,90 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -865,10 +845,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:BE78"/>
+  <dimension ref="A2:BE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34:C35"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,1067 +860,1067 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="33"/>
-      <c r="V2" s="33"/>
-      <c r="W2" s="33"/>
-      <c r="X2" s="33"/>
-      <c r="Y2" s="33"/>
-      <c r="Z2" s="33"/>
-      <c r="AA2" s="33"/>
-      <c r="AB2" s="33"/>
-      <c r="AC2" s="33"/>
-      <c r="AD2" s="33"/>
-      <c r="AE2" s="33"/>
-      <c r="AF2" s="33"/>
-      <c r="AG2" s="33"/>
-      <c r="AH2" s="33"/>
-      <c r="AI2" s="33"/>
-      <c r="AJ2" s="33"/>
-      <c r="AK2" s="33"/>
-      <c r="AL2" s="33"/>
-      <c r="AM2" s="33"/>
-      <c r="AN2" s="33"/>
-      <c r="AO2" s="33"/>
-      <c r="AP2" s="33"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="36"/>
+      <c r="Z2" s="36"/>
+      <c r="AA2" s="36"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="36"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="36"/>
+      <c r="AK2" s="36"/>
+      <c r="AL2" s="36"/>
+      <c r="AM2" s="36"/>
+      <c r="AN2" s="36"/>
+      <c r="AO2" s="36"/>
+      <c r="AP2" s="36"/>
     </row>
     <row r="3" spans="1:57" ht="18" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37"/>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
-      <c r="T3" s="37"/>
-      <c r="U3" s="37"/>
-      <c r="V3" s="37"/>
-      <c r="W3" s="37"/>
-      <c r="X3" s="37"/>
-      <c r="Y3" s="37"/>
-      <c r="Z3" s="37"/>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37"/>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37"/>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="37"/>
-      <c r="AM3" s="37"/>
-      <c r="AN3" s="37"/>
-      <c r="AO3" s="37"/>
-      <c r="AP3" s="37"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="39"/>
+      <c r="AM3" s="39"/>
+      <c r="AN3" s="39"/>
+      <c r="AO3" s="39"/>
+      <c r="AP3" s="39"/>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B4" s="35"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="36" t="s">
+      <c r="B4" s="37"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36" t="s">
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="36"/>
-      <c r="AF4" s="36"/>
-      <c r="AG4" s="36"/>
-      <c r="AH4" s="36"/>
-      <c r="AI4" s="36"/>
-      <c r="AJ4" s="36"/>
-      <c r="AK4" s="36"/>
-      <c r="AL4" s="36"/>
-      <c r="AM4" s="36"/>
-      <c r="AN4" s="36"/>
-      <c r="AO4" s="36"/>
-      <c r="AP4" s="36"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="38"/>
+      <c r="Q4" s="38"/>
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
+      <c r="Y4" s="38"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="38"/>
+      <c r="AB4" s="38"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="38"/>
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="38"/>
+      <c r="AI4" s="38"/>
+      <c r="AJ4" s="38"/>
+      <c r="AK4" s="38"/>
+      <c r="AL4" s="38"/>
+      <c r="AM4" s="38"/>
+      <c r="AN4" s="38"/>
+      <c r="AO4" s="38"/>
+      <c r="AP4" s="38"/>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B5" s="35"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="32">
+      <c r="B5" s="37"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="23">
         <v>23</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="23">
         <v>24</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="23">
         <v>25</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="23">
         <v>26</v>
       </c>
-      <c r="H5" s="32">
+      <c r="H5" s="23">
         <v>27</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="23">
         <v>28</v>
       </c>
-      <c r="J5" s="32">
+      <c r="J5" s="23">
         <v>29</v>
       </c>
-      <c r="K5" s="32">
+      <c r="K5" s="23">
         <v>30</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="23">
         <v>31</v>
       </c>
-      <c r="M5" s="32">
+      <c r="M5" s="23">
         <v>1</v>
       </c>
-      <c r="N5" s="32">
+      <c r="N5" s="23">
         <v>2</v>
       </c>
-      <c r="O5" s="32">
+      <c r="O5" s="23">
         <v>3</v>
       </c>
-      <c r="P5" s="32">
+      <c r="P5" s="23">
         <v>4</v>
       </c>
-      <c r="Q5" s="32">
+      <c r="Q5" s="23">
         <v>5</v>
       </c>
-      <c r="R5" s="32">
+      <c r="R5" s="23">
         <v>6</v>
       </c>
-      <c r="S5" s="32">
+      <c r="S5" s="23">
         <v>7</v>
       </c>
-      <c r="T5" s="32">
+      <c r="T5" s="23">
         <v>8</v>
       </c>
-      <c r="U5" s="32">
+      <c r="U5" s="23">
         <v>9</v>
       </c>
-      <c r="V5" s="32">
+      <c r="V5" s="23">
         <v>10</v>
       </c>
-      <c r="W5" s="32">
+      <c r="W5" s="23">
         <v>11</v>
       </c>
-      <c r="X5" s="32">
+      <c r="X5" s="23">
         <v>12</v>
       </c>
-      <c r="Y5" s="32">
+      <c r="Y5" s="23">
         <v>13</v>
       </c>
-      <c r="Z5" s="32">
+      <c r="Z5" s="23">
         <v>14</v>
       </c>
-      <c r="AA5" s="32">
+      <c r="AA5" s="23">
         <v>15</v>
       </c>
-      <c r="AB5" s="32">
+      <c r="AB5" s="23">
         <v>16</v>
       </c>
-      <c r="AC5" s="32">
+      <c r="AC5" s="23">
         <v>17</v>
       </c>
-      <c r="AD5" s="32">
+      <c r="AD5" s="23">
         <v>18</v>
       </c>
-      <c r="AE5" s="32">
+      <c r="AE5" s="23">
         <v>19</v>
       </c>
-      <c r="AF5" s="32">
+      <c r="AF5" s="23">
         <v>20</v>
       </c>
-      <c r="AG5" s="32">
+      <c r="AG5" s="23">
         <v>21</v>
       </c>
-      <c r="AH5" s="32">
+      <c r="AH5" s="23">
         <v>22</v>
       </c>
-      <c r="AI5" s="32">
+      <c r="AI5" s="23">
         <v>23</v>
       </c>
-      <c r="AJ5" s="32">
+      <c r="AJ5" s="23">
         <v>24</v>
       </c>
-      <c r="AK5" s="32">
+      <c r="AK5" s="23">
         <v>25</v>
       </c>
-      <c r="AL5" s="32">
+      <c r="AL5" s="23">
         <v>26</v>
       </c>
-      <c r="AM5" s="32">
+      <c r="AM5" s="23">
         <v>27</v>
       </c>
-      <c r="AN5" s="32">
+      <c r="AN5" s="23">
         <v>28</v>
       </c>
-      <c r="AO5" s="32">
+      <c r="AO5" s="23">
         <v>29</v>
       </c>
-      <c r="AP5" s="32">
+      <c r="AP5" s="23">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="9"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-      <c r="AC6" s="9"/>
-      <c r="AD6" s="9"/>
-      <c r="AE6" s="8"/>
-      <c r="AF6" s="9"/>
-      <c r="AG6" s="9"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="9"/>
-      <c r="AK6" s="9"/>
-      <c r="AL6" s="9"/>
-      <c r="AM6" s="9"/>
-      <c r="AN6" s="9"/>
-      <c r="AO6" s="9"/>
-      <c r="AP6" s="9"/>
-      <c r="AQ6" s="11"/>
-      <c r="AR6" s="11"/>
-      <c r="AS6" s="11"/>
-      <c r="AT6" s="11"/>
-      <c r="AU6" s="11"/>
-      <c r="AV6" s="11"/>
-      <c r="AW6" s="11"/>
-      <c r="AX6" s="11"/>
-      <c r="AY6" s="11"/>
-      <c r="AZ6" s="11"/>
-      <c r="BA6" s="11"/>
-      <c r="BB6" s="11"/>
-      <c r="BC6" s="11"/>
-      <c r="BD6" s="11"/>
-      <c r="BE6" s="11"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7"/>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
+      <c r="AN6" s="7"/>
+      <c r="AO6" s="7"/>
+      <c r="AP6" s="7"/>
+      <c r="AQ6" s="9"/>
+      <c r="AR6" s="9"/>
+      <c r="AS6" s="9"/>
+      <c r="AT6" s="9"/>
+      <c r="AU6" s="9"/>
+      <c r="AV6" s="9"/>
+      <c r="AW6" s="9"/>
+      <c r="AX6" s="9"/>
+      <c r="AY6" s="9"/>
+      <c r="AZ6" s="9"/>
+      <c r="BA6" s="9"/>
+      <c r="BB6" s="9"/>
+      <c r="BC6" s="9"/>
+      <c r="BD6" s="9"/>
+      <c r="BE6" s="9"/>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B7" s="22" t="s">
-        <v>30</v>
+      <c r="B7" s="18" t="s">
+        <v>47</v>
       </c>
       <c r="C7" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="29"/>
+      <c r="D7" s="20"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="5"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="7"/>
+      <c r="P7" s="8"/>
+      <c r="Q7" s="5"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
-      <c r="W7" s="10"/>
-      <c r="X7" s="7"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="5"/>
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
       <c r="AB7" s="2"/>
       <c r="AC7" s="2"/>
-      <c r="AD7" s="10"/>
-      <c r="AE7" s="7"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="5"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="2"/>
       <c r="AH7" s="2"/>
       <c r="AI7" s="2"/>
       <c r="AJ7" s="2"/>
-      <c r="AK7" s="10"/>
-      <c r="AL7" s="10"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
       <c r="AM7" s="2"/>
       <c r="AN7" s="2"/>
       <c r="AO7" s="2"/>
       <c r="AP7" s="2"/>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B8" s="4" t="s">
-        <v>31</v>
+      <c r="B8" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="C8" s="42"/>
-      <c r="D8" s="29"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="7"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-      <c r="P8" s="10"/>
-      <c r="Q8" s="7"/>
+      <c r="P8" s="8"/>
+      <c r="Q8" s="5"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="7"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="5"/>
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
       <c r="AA8" s="2"/>
       <c r="AB8" s="2"/>
       <c r="AC8" s="2"/>
-      <c r="AD8" s="10"/>
-      <c r="AE8" s="7"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="5"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="2"/>
       <c r="AH8" s="2"/>
       <c r="AI8" s="2"/>
       <c r="AJ8" s="2"/>
-      <c r="AK8" s="10"/>
-      <c r="AL8" s="10"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
       <c r="AM8" s="2"/>
       <c r="AN8" s="2"/>
       <c r="AO8" s="2"/>
       <c r="AP8" s="2"/>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B9" s="22" t="s">
-        <v>32</v>
+      <c r="B9" s="27" t="s">
+        <v>45</v>
       </c>
       <c r="C9" s="43"/>
-      <c r="D9" s="29"/>
+      <c r="D9" s="20"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="5"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="7"/>
+      <c r="P9" s="8"/>
+      <c r="Q9" s="5"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
       <c r="V9" s="2"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="7"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="5"/>
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
       <c r="AA9" s="2"/>
       <c r="AB9" s="2"/>
       <c r="AC9" s="2"/>
-      <c r="AD9" s="10"/>
-      <c r="AE9" s="7"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="5"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="2"/>
       <c r="AH9" s="2"/>
       <c r="AI9" s="2"/>
       <c r="AJ9" s="2"/>
-      <c r="AK9" s="10"/>
-      <c r="AL9" s="10"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
       <c r="AM9" s="2"/>
       <c r="AN9" s="2"/>
       <c r="AO9" s="2"/>
       <c r="AP9" s="2"/>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="44" t="s">
+      <c r="C10" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
       <c r="F10" s="1"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="7"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="5"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
-      <c r="P10" s="10"/>
-      <c r="Q10" s="7"/>
+      <c r="P10" s="8"/>
+      <c r="Q10" s="5"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2"/>
       <c r="V10" s="2"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="7"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="5"/>
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
       <c r="AA10" s="2"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="7"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="5"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="2"/>
       <c r="AH10" s="2"/>
       <c r="AI10" s="2"/>
       <c r="AJ10" s="2"/>
-      <c r="AK10" s="10"/>
-      <c r="AL10" s="10"/>
+      <c r="AK10" s="8"/>
+      <c r="AL10" s="8"/>
       <c r="AM10" s="2"/>
       <c r="AN10" s="2"/>
       <c r="AO10" s="2"/>
       <c r="AP10" s="2"/>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
+      <c r="A11" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="32"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="1"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="7"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="5"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="7"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="5"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="2"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="7"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="5"/>
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
-      <c r="AD11" s="10"/>
-      <c r="AE11" s="7"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="5"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="2"/>
       <c r="AH11" s="2"/>
       <c r="AI11" s="2"/>
       <c r="AJ11" s="2"/>
-      <c r="AK11" s="10"/>
-      <c r="AL11" s="10"/>
+      <c r="AK11" s="8"/>
+      <c r="AL11" s="8"/>
       <c r="AM11" s="2"/>
       <c r="AN11" s="2"/>
       <c r="AO11" s="2"/>
       <c r="AP11" s="2"/>
     </row>
     <row r="12" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="41" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="7"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="5"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="7"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="5"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="7"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="5"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
       <c r="AA12" s="2"/>
       <c r="AB12" s="2"/>
       <c r="AC12" s="2"/>
-      <c r="AD12" s="10"/>
-      <c r="AE12" s="7"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="5"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="2"/>
       <c r="AH12" s="2"/>
       <c r="AI12" s="2"/>
       <c r="AJ12" s="2"/>
-      <c r="AK12" s="10"/>
-      <c r="AL12" s="10"/>
+      <c r="AK12" s="8"/>
+      <c r="AL12" s="8"/>
       <c r="AM12" s="2"/>
       <c r="AN12" s="2"/>
       <c r="AO12" s="2"/>
       <c r="AP12" s="2"/>
     </row>
     <row r="13" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="42"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="7"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="5"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="7"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="5"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="7"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="5"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
       <c r="AA13" s="2"/>
       <c r="AB13" s="2"/>
       <c r="AC13" s="2"/>
-      <c r="AD13" s="10"/>
-      <c r="AE13" s="7"/>
+      <c r="AD13" s="8"/>
+      <c r="AE13" s="5"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="2"/>
       <c r="AH13" s="2"/>
       <c r="AI13" s="2"/>
       <c r="AJ13" s="2"/>
-      <c r="AK13" s="10"/>
-      <c r="AL13" s="10"/>
+      <c r="AK13" s="8"/>
+      <c r="AL13" s="8"/>
       <c r="AM13" s="2"/>
       <c r="AN13" s="2"/>
       <c r="AO13" s="2"/>
       <c r="AP13" s="2"/>
     </row>
     <row r="14" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="7"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="5"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="7"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="5"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="7"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="5"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="2"/>
       <c r="AC14" s="2"/>
-      <c r="AD14" s="10"/>
-      <c r="AE14" s="7"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="5"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="2"/>
       <c r="AH14" s="2"/>
       <c r="AI14" s="2"/>
       <c r="AJ14" s="2"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="10"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
       <c r="AM14" s="2"/>
       <c r="AN14" s="2"/>
       <c r="AO14" s="2"/>
       <c r="AP14" s="2"/>
     </row>
     <row r="15" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="2"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="7"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="5"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="7"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="5"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="7"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="5"/>
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
       <c r="AA15" s="2"/>
       <c r="AB15" s="2"/>
       <c r="AC15" s="2"/>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="7"/>
+      <c r="AD15" s="8"/>
+      <c r="AE15" s="5"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="2"/>
       <c r="AH15" s="2"/>
       <c r="AI15" s="2"/>
       <c r="AJ15" s="2"/>
-      <c r="AK15" s="10"/>
-      <c r="AL15" s="10"/>
+      <c r="AK15" s="8"/>
+      <c r="AL15" s="8"/>
       <c r="AM15" s="2"/>
       <c r="AN15" s="2"/>
       <c r="AO15" s="2"/>
       <c r="AP15" s="2"/>
     </row>
     <row r="16" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="17" t="s">
         <v>29</v>
       </c>
       <c r="C16" s="43"/>
       <c r="D16" s="2"/>
-      <c r="E16" s="29"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="7"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="5"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="7"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="5"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
       <c r="T16" s="2"/>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="7"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="5"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
       <c r="AB16" s="2"/>
       <c r="AC16" s="2"/>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="7"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="5"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="2"/>
       <c r="AH16" s="2"/>
       <c r="AI16" s="2"/>
       <c r="AJ16" s="2"/>
-      <c r="AK16" s="10"/>
-      <c r="AL16" s="10"/>
+      <c r="AK16" s="8"/>
+      <c r="AL16" s="8"/>
       <c r="AM16" s="2"/>
       <c r="AN16" s="2"/>
       <c r="AO16" s="2"/>
       <c r="AP16" s="2"/>
     </row>
     <row r="17" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="46" t="s">
+      <c r="C17" s="33" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="29"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="20"/>
       <c r="H17" s="1"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="7"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="5"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="7"/>
+      <c r="P17" s="8"/>
+      <c r="Q17" s="5"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="7"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="5"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="7"/>
+      <c r="AD17" s="8"/>
+      <c r="AE17" s="5"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="2"/>
       <c r="AH17" s="2"/>
       <c r="AI17" s="2"/>
       <c r="AJ17" s="2"/>
-      <c r="AK17" s="10"/>
-      <c r="AL17" s="10"/>
+      <c r="AK17" s="8"/>
+      <c r="AL17" s="8"/>
       <c r="AM17" s="2"/>
       <c r="AN17" s="2"/>
       <c r="AO17" s="2"/>
       <c r="AP17" s="2"/>
     </row>
     <row r="18" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B18" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="47"/>
+      <c r="B18" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="34"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="29"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="7"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="5"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="7"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="5"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2"/>
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="7"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="5"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="7"/>
+      <c r="AD18" s="8"/>
+      <c r="AE18" s="5"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="2"/>
       <c r="AH18" s="2"/>
       <c r="AI18" s="2"/>
       <c r="AJ18" s="2"/>
-      <c r="AK18" s="10"/>
-      <c r="AL18" s="10"/>
+      <c r="AK18" s="8"/>
+      <c r="AL18" s="8"/>
       <c r="AM18" s="2"/>
       <c r="AN18" s="2"/>
       <c r="AO18" s="2"/>
       <c r="AP18" s="2"/>
     </row>
     <row r="19" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B19" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="48"/>
+      <c r="B19" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="35"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="29"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="7"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="5"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="7"/>
+      <c r="P19" s="8"/>
+      <c r="Q19" s="5"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="7"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="5"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
       <c r="AB19" s="2"/>
       <c r="AC19" s="2"/>
-      <c r="AD19" s="10"/>
-      <c r="AE19" s="7"/>
+      <c r="AD19" s="8"/>
+      <c r="AE19" s="5"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="2"/>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
       <c r="AJ19" s="2"/>
-      <c r="AK19" s="10"/>
-      <c r="AL19" s="10"/>
+      <c r="AK19" s="8"/>
+      <c r="AL19" s="8"/>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2"/>
       <c r="AO19" s="2"/>
       <c r="AP19" s="2"/>
     </row>
     <row r="20" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="44" t="s">
+      <c r="C20" s="30" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="7"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="20"/>
+      <c r="J20" s="5"/>
       <c r="K20" s="1"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
-      <c r="N20" s="10"/>
+      <c r="N20" s="8"/>
       <c r="O20" s="2"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="7"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="5"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
       <c r="T20" s="2"/>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="7"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="5"/>
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
       <c r="AB20" s="2"/>
       <c r="AC20" s="2"/>
-      <c r="AD20" s="10"/>
-      <c r="AE20" s="7"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="5"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
       <c r="AJ20" s="2"/>
-      <c r="AK20" s="10"/>
-      <c r="AL20" s="10"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
       <c r="AM20" s="2"/>
       <c r="AN20" s="2"/>
       <c r="AO20" s="2"/>
       <c r="AP20" s="2"/>
     </row>
     <row r="21" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B21" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="49"/>
+      <c r="B21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="31"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="7"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="5"/>
       <c r="K21" s="1"/>
       <c r="L21" s="2"/>
       <c r="M21" s="2"/>
-      <c r="N21" s="10"/>
+      <c r="N21" s="8"/>
       <c r="O21" s="2"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="7"/>
+      <c r="P21" s="8"/>
+      <c r="Q21" s="5"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
-      <c r="W21" s="10"/>
-      <c r="X21" s="7"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="5"/>
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
       <c r="AB21" s="2"/>
       <c r="AC21" s="2"/>
-      <c r="AD21" s="10"/>
-      <c r="AE21" s="7"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="5"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="2"/>
       <c r="AH21" s="2"/>
       <c r="AI21" s="2"/>
       <c r="AJ21" s="2"/>
-      <c r="AK21" s="10"/>
-      <c r="AL21" s="10"/>
+      <c r="AK21" s="8"/>
+      <c r="AL21" s="8"/>
       <c r="AM21" s="2"/>
       <c r="AN21" s="2"/>
       <c r="AO21" s="2"/>
       <c r="AP21" s="2"/>
     </row>
     <row r="22" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="A22" s="23"/>
-      <c r="B22" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C22" s="45"/>
+      <c r="A22" s="19"/>
+      <c r="B22" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="32"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="7"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="5"/>
       <c r="K22" s="1"/>
       <c r="L22" s="2"/>
       <c r="M22" s="2"/>
-      <c r="N22" s="10"/>
+      <c r="N22" s="8"/>
       <c r="O22" s="2"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="7"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="5"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
       <c r="T22" s="2"/>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="7"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="5"/>
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2"/>
       <c r="AC22" s="2"/>
-      <c r="AD22" s="10"/>
-      <c r="AE22" s="7"/>
+      <c r="AD22" s="8"/>
+      <c r="AE22" s="5"/>
       <c r="AF22" s="2"/>
       <c r="AG22" s="2"/>
       <c r="AH22" s="2"/>
       <c r="AI22" s="2"/>
       <c r="AJ22" s="2"/>
-      <c r="AK22" s="10"/>
-      <c r="AL22" s="10"/>
+      <c r="AK22" s="8"/>
+      <c r="AL22" s="8"/>
       <c r="AM22" s="2"/>
       <c r="AN22" s="2"/>
       <c r="AO22" s="2"/>
       <c r="AP22" s="2"/>
     </row>
     <row r="23" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="46" t="s">
+      <c r="C23" s="33" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="2"/>
@@ -1948,189 +1928,189 @@
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="10"/>
+      <c r="N23" s="8"/>
       <c r="O23" s="2"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="7"/>
+      <c r="P23" s="8"/>
+      <c r="Q23" s="5"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
       <c r="T23" s="2"/>
       <c r="U23" s="2"/>
       <c r="V23" s="2"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="7"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="5"/>
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2"/>
-      <c r="AD23" s="10"/>
-      <c r="AE23" s="7"/>
+      <c r="AD23" s="8"/>
+      <c r="AE23" s="5"/>
       <c r="AF23" s="2"/>
       <c r="AG23" s="2"/>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
       <c r="AJ23" s="2"/>
-      <c r="AK23" s="10"/>
-      <c r="AL23" s="10"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2"/>
       <c r="AO23" s="2"/>
       <c r="AP23" s="2"/>
     </row>
     <row r="24" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="47"/>
+      <c r="B24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="34"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
       <c r="M24" s="1"/>
-      <c r="N24" s="10"/>
+      <c r="N24" s="8"/>
       <c r="O24" s="2"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="7"/>
+      <c r="P24" s="8"/>
+      <c r="Q24" s="5"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
       <c r="T24" s="2"/>
       <c r="U24" s="2"/>
       <c r="V24" s="2"/>
-      <c r="W24" s="10"/>
-      <c r="X24" s="7"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="5"/>
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
       <c r="AA24" s="2"/>
       <c r="AB24" s="2"/>
       <c r="AC24" s="2"/>
-      <c r="AD24" s="10"/>
-      <c r="AE24" s="7"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="5"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="2"/>
       <c r="AH24" s="2"/>
       <c r="AI24" s="2"/>
       <c r="AJ24" s="2"/>
-      <c r="AK24" s="10"/>
-      <c r="AL24" s="10"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="8"/>
       <c r="AM24" s="2"/>
       <c r="AN24" s="2"/>
       <c r="AO24" s="2"/>
       <c r="AP24" s="2"/>
     </row>
     <row r="25" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="48"/>
+      <c r="B25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="35"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="10"/>
+      <c r="N25" s="8"/>
       <c r="O25" s="2"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="7"/>
+      <c r="P25" s="8"/>
+      <c r="Q25" s="5"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
       <c r="V25" s="2"/>
-      <c r="W25" s="10"/>
-      <c r="X25" s="7"/>
+      <c r="W25" s="8"/>
+      <c r="X25" s="5"/>
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
       <c r="AA25" s="2"/>
       <c r="AB25" s="2"/>
       <c r="AC25" s="2"/>
-      <c r="AD25" s="10"/>
-      <c r="AE25" s="7"/>
+      <c r="AD25" s="8"/>
+      <c r="AE25" s="5"/>
       <c r="AF25" s="2"/>
       <c r="AG25" s="2"/>
       <c r="AH25" s="2"/>
       <c r="AI25" s="2"/>
       <c r="AJ25" s="2"/>
-      <c r="AK25" s="10"/>
-      <c r="AL25" s="10"/>
+      <c r="AK25" s="8"/>
+      <c r="AL25" s="8"/>
       <c r="AM25" s="2"/>
       <c r="AN25" s="2"/>
       <c r="AO25" s="2"/>
       <c r="AP25" s="2"/>
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B26" s="40" t="s">
+      <c r="B26" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="10"/>
-      <c r="I26" s="10"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="16"/>
-      <c r="Z26" s="16"/>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="16"/>
-      <c r="AC26" s="16"/>
-      <c r="AD26" s="10"/>
-      <c r="AE26" s="7"/>
-      <c r="AF26" s="10"/>
-      <c r="AG26" s="10"/>
-      <c r="AH26" s="10"/>
-      <c r="AI26" s="10"/>
-      <c r="AJ26" s="10"/>
-      <c r="AK26" s="10"/>
-      <c r="AL26" s="10"/>
-      <c r="AM26" s="10"/>
-      <c r="AN26" s="10"/>
-      <c r="AO26" s="10"/>
-      <c r="AP26" s="10"/>
-      <c r="AQ26" s="11"/>
-      <c r="AR26" s="11"/>
-      <c r="AS26" s="11"/>
-      <c r="AT26" s="11"/>
-      <c r="AU26" s="11"/>
-      <c r="AV26" s="11"/>
-      <c r="AW26" s="11"/>
-      <c r="AX26" s="11"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="8"/>
+      <c r="L26" s="8"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+      <c r="Y26" s="12"/>
+      <c r="Z26" s="12"/>
+      <c r="AA26" s="12"/>
+      <c r="AB26" s="12"/>
+      <c r="AC26" s="12"/>
+      <c r="AD26" s="8"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="8"/>
+      <c r="AG26" s="8"/>
+      <c r="AH26" s="8"/>
+      <c r="AI26" s="8"/>
+      <c r="AJ26" s="8"/>
+      <c r="AK26" s="8"/>
+      <c r="AL26" s="8"/>
+      <c r="AM26" s="8"/>
+      <c r="AN26" s="8"/>
+      <c r="AO26" s="8"/>
+      <c r="AP26" s="8"/>
+      <c r="AQ26" s="9"/>
+      <c r="AR26" s="9"/>
+      <c r="AS26" s="9"/>
+      <c r="AT26" s="9"/>
+      <c r="AU26" s="9"/>
+      <c r="AV26" s="9"/>
+      <c r="AW26" s="9"/>
+      <c r="AX26" s="9"/>
     </row>
     <row r="27" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="50" t="s">
+      <c r="C27" s="46" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="2"/>
@@ -2138,171 +2118,171 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="10"/>
-      <c r="J27" s="7"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="5"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="29"/>
-      <c r="N27" s="29"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
-      <c r="Q27" s="7"/>
+      <c r="Q27" s="5"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
       <c r="T27" s="2"/>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="7"/>
+      <c r="W27" s="8"/>
+      <c r="X27" s="5"/>
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
       <c r="AB27" s="2"/>
       <c r="AC27" s="2"/>
-      <c r="AD27" s="10"/>
-      <c r="AE27" s="7"/>
+      <c r="AD27" s="8"/>
+      <c r="AE27" s="5"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="2"/>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
       <c r="AJ27" s="2"/>
-      <c r="AK27" s="10"/>
-      <c r="AL27" s="10"/>
+      <c r="AK27" s="8"/>
+      <c r="AL27" s="8"/>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2"/>
       <c r="AO27" s="2"/>
       <c r="AP27" s="2"/>
     </row>
     <row r="28" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" s="51"/>
+      <c r="B28" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="47"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="10"/>
-      <c r="J28" s="7"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="5"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
-      <c r="Q28" s="7"/>
+      <c r="Q28" s="5"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
       <c r="T28" s="2"/>
       <c r="U28" s="2"/>
       <c r="V28" s="2"/>
-      <c r="W28" s="10"/>
-      <c r="X28" s="7"/>
+      <c r="W28" s="8"/>
+      <c r="X28" s="5"/>
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
       <c r="AA28" s="2"/>
       <c r="AB28" s="2"/>
       <c r="AC28" s="2"/>
-      <c r="AD28" s="10"/>
-      <c r="AE28" s="7"/>
+      <c r="AD28" s="8"/>
+      <c r="AE28" s="5"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="2"/>
       <c r="AH28" s="2"/>
       <c r="AI28" s="2"/>
       <c r="AJ28" s="2"/>
-      <c r="AK28" s="10"/>
-      <c r="AL28" s="10"/>
+      <c r="AK28" s="8"/>
+      <c r="AL28" s="8"/>
       <c r="AM28" s="2"/>
       <c r="AN28" s="2"/>
       <c r="AO28" s="2"/>
       <c r="AP28" s="2"/>
     </row>
     <row r="29" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="51"/>
+      <c r="B29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="47"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="7"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="5"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="29"/>
-      <c r="N29" s="29"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
       <c r="O29" s="1"/>
       <c r="P29" s="1"/>
-      <c r="Q29" s="7"/>
+      <c r="Q29" s="5"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
-      <c r="W29" s="10"/>
-      <c r="X29" s="7"/>
+      <c r="W29" s="8"/>
+      <c r="X29" s="5"/>
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
       <c r="AB29" s="2"/>
       <c r="AC29" s="2"/>
-      <c r="AD29" s="10"/>
-      <c r="AE29" s="7"/>
+      <c r="AD29" s="8"/>
+      <c r="AE29" s="5"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="2"/>
       <c r="AH29" s="2"/>
       <c r="AI29" s="2"/>
       <c r="AJ29" s="2"/>
-      <c r="AK29" s="10"/>
-      <c r="AL29" s="10"/>
+      <c r="AK29" s="8"/>
+      <c r="AL29" s="8"/>
       <c r="AM29" s="2"/>
       <c r="AN29" s="2"/>
       <c r="AO29" s="2"/>
       <c r="AP29" s="2"/>
     </row>
     <row r="30" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C30" s="51"/>
+      <c r="B30" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="47"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="7"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="5"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="29"/>
-      <c r="N30" s="29"/>
+      <c r="M30" s="20"/>
+      <c r="N30" s="20"/>
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
-      <c r="Q30" s="7"/>
+      <c r="Q30" s="5"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
       <c r="V30" s="2"/>
-      <c r="W30" s="10"/>
-      <c r="X30" s="7"/>
+      <c r="W30" s="8"/>
+      <c r="X30" s="5"/>
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
       <c r="AB30" s="2"/>
       <c r="AC30" s="2"/>
-      <c r="AD30" s="10"/>
-      <c r="AE30" s="7"/>
+      <c r="AD30" s="8"/>
+      <c r="AE30" s="5"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="2"/>
       <c r="AH30" s="2"/>
       <c r="AI30" s="2"/>
       <c r="AJ30" s="2"/>
-      <c r="AK30" s="10"/>
-      <c r="AL30" s="10"/>
+      <c r="AK30" s="8"/>
+      <c r="AL30" s="8"/>
       <c r="AM30" s="2"/>
       <c r="AN30" s="2"/>
       <c r="AO30" s="2"/>
@@ -2310,57 +2290,57 @@
     </row>
     <row r="31" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="52"/>
+        <v>31</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="48"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="7"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="5"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="29"/>
-      <c r="N31" s="29"/>
+      <c r="M31" s="20"/>
+      <c r="N31" s="20"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
-      <c r="Q31" s="7"/>
+      <c r="Q31" s="5"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
       <c r="T31" s="2"/>
       <c r="U31" s="2"/>
       <c r="V31" s="2"/>
-      <c r="W31" s="10"/>
-      <c r="X31" s="7"/>
+      <c r="W31" s="8"/>
+      <c r="X31" s="5"/>
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
       <c r="AA31" s="2"/>
       <c r="AB31" s="2"/>
       <c r="AC31" s="2"/>
-      <c r="AD31" s="10"/>
-      <c r="AE31" s="7"/>
+      <c r="AD31" s="8"/>
+      <c r="AE31" s="5"/>
       <c r="AF31" s="2"/>
       <c r="AG31" s="2"/>
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
       <c r="AJ31" s="2"/>
-      <c r="AK31" s="10"/>
-      <c r="AL31" s="10"/>
+      <c r="AK31" s="8"/>
+      <c r="AL31" s="8"/>
       <c r="AM31" s="2"/>
       <c r="AN31" s="2"/>
       <c r="AO31" s="2"/>
       <c r="AP31" s="2"/>
     </row>
     <row r="32" spans="1:50" x14ac:dyDescent="0.25">
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="53" t="s">
+      <c r="C32" s="49" t="s">
         <v>10</v>
       </c>
       <c r="D32" s="2"/>
@@ -2368,91 +2348,91 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="10"/>
-      <c r="J32" s="7"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="5"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="29"/>
-      <c r="N32" s="29"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="20"/>
       <c r="O32" s="1"/>
-      <c r="P32" s="10"/>
-      <c r="Q32" s="7"/>
+      <c r="P32" s="8"/>
+      <c r="Q32" s="5"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="2"/>
       <c r="V32" s="2"/>
-      <c r="W32" s="10"/>
-      <c r="X32" s="7"/>
+      <c r="W32" s="8"/>
+      <c r="X32" s="5"/>
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
       <c r="AA32" s="2"/>
       <c r="AB32" s="2"/>
       <c r="AC32" s="2"/>
-      <c r="AD32" s="10"/>
-      <c r="AE32" s="7"/>
+      <c r="AD32" s="8"/>
+      <c r="AE32" s="5"/>
       <c r="AF32" s="2"/>
       <c r="AG32" s="2"/>
       <c r="AH32" s="2"/>
       <c r="AI32" s="2"/>
       <c r="AJ32" s="2"/>
-      <c r="AK32" s="10"/>
-      <c r="AL32" s="10"/>
+      <c r="AK32" s="8"/>
+      <c r="AL32" s="8"/>
       <c r="AM32" s="2"/>
       <c r="AN32" s="2"/>
       <c r="AO32" s="2"/>
       <c r="AP32" s="2"/>
     </row>
     <row r="33" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B33" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" s="54"/>
+      <c r="B33" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="50"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="10"/>
-      <c r="J33" s="7"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="5"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="29"/>
-      <c r="N33" s="29"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
       <c r="O33" s="1"/>
-      <c r="P33" s="10"/>
-      <c r="Q33" s="7"/>
+      <c r="P33" s="8"/>
+      <c r="Q33" s="5"/>
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
       <c r="U33" s="2"/>
       <c r="V33" s="2"/>
-      <c r="W33" s="10"/>
-      <c r="X33" s="7"/>
+      <c r="W33" s="8"/>
+      <c r="X33" s="5"/>
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
       <c r="AA33" s="2"/>
       <c r="AB33" s="2"/>
       <c r="AC33" s="2"/>
-      <c r="AD33" s="10"/>
-      <c r="AE33" s="7"/>
+      <c r="AD33" s="8"/>
+      <c r="AE33" s="5"/>
       <c r="AF33" s="2"/>
       <c r="AG33" s="2"/>
       <c r="AH33" s="2"/>
       <c r="AI33" s="2"/>
       <c r="AJ33" s="2"/>
-      <c r="AK33" s="10"/>
-      <c r="AL33" s="10"/>
+      <c r="AK33" s="8"/>
+      <c r="AL33" s="8"/>
       <c r="AM33" s="2"/>
       <c r="AN33" s="2"/>
       <c r="AO33" s="2"/>
       <c r="AP33" s="2"/>
     </row>
     <row r="34" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="55" t="s">
+      <c r="C34" s="44" t="s">
         <v>11</v>
       </c>
       <c r="D34" s="2"/>
@@ -2460,91 +2440,91 @@
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="7"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="5"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
-      <c r="O34" s="29"/>
-      <c r="P34" s="29"/>
-      <c r="Q34" s="19"/>
-      <c r="R34" s="29"/>
+      <c r="O34" s="51"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="20"/>
       <c r="S34" s="2"/>
       <c r="T34" s="2"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
-      <c r="X34" s="7"/>
+      <c r="X34" s="5"/>
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
       <c r="AA34" s="2"/>
       <c r="AB34" s="2"/>
       <c r="AC34" s="2"/>
-      <c r="AD34" s="10"/>
-      <c r="AE34" s="7"/>
+      <c r="AD34" s="8"/>
+      <c r="AE34" s="5"/>
       <c r="AF34" s="2"/>
       <c r="AG34" s="2"/>
       <c r="AH34" s="2"/>
       <c r="AI34" s="2"/>
       <c r="AJ34" s="2"/>
-      <c r="AK34" s="10"/>
-      <c r="AL34" s="10"/>
+      <c r="AK34" s="8"/>
+      <c r="AL34" s="8"/>
       <c r="AM34" s="2"/>
       <c r="AN34" s="2"/>
       <c r="AO34" s="2"/>
       <c r="AP34" s="2"/>
     </row>
     <row r="35" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B35" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C35" s="56"/>
+      <c r="B35" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" s="45"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="7"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="5"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
-      <c r="O35" s="29"/>
-      <c r="P35" s="29"/>
-      <c r="Q35" s="19"/>
-      <c r="R35" s="29"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="15"/>
+      <c r="R35" s="20"/>
       <c r="S35" s="2"/>
       <c r="T35" s="2"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="7"/>
+      <c r="X35" s="5"/>
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
       <c r="AC35" s="2"/>
-      <c r="AD35" s="10"/>
-      <c r="AE35" s="7"/>
+      <c r="AD35" s="8"/>
+      <c r="AE35" s="5"/>
       <c r="AF35" s="2"/>
       <c r="AG35" s="2"/>
       <c r="AH35" s="2"/>
       <c r="AI35" s="2"/>
       <c r="AJ35" s="2"/>
-      <c r="AK35" s="10"/>
-      <c r="AL35" s="10"/>
+      <c r="AK35" s="8"/>
+      <c r="AL35" s="8"/>
       <c r="AM35" s="2"/>
       <c r="AN35" s="2"/>
       <c r="AO35" s="2"/>
       <c r="AP35" s="2"/>
     </row>
     <row r="36" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="57" t="s">
+      <c r="C36" s="24" t="s">
         <v>19</v>
       </c>
       <c r="D36" s="2"/>
@@ -2552,46 +2532,46 @@
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="7"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="5"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
-      <c r="P36" s="10"/>
-      <c r="Q36" s="7"/>
+      <c r="P36" s="8"/>
+      <c r="Q36" s="5"/>
       <c r="R36" s="2"/>
-      <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
-      <c r="U36" s="29"/>
-      <c r="V36" s="29"/>
-      <c r="W36" s="29"/>
-      <c r="X36" s="7"/>
+      <c r="S36" s="20"/>
+      <c r="T36" s="20"/>
+      <c r="U36" s="20"/>
+      <c r="V36" s="20"/>
+      <c r="W36" s="20"/>
+      <c r="X36" s="5"/>
       <c r="Y36" s="1"/>
       <c r="Z36" s="1"/>
       <c r="AA36" s="1"/>
       <c r="AB36" s="1"/>
       <c r="AC36" s="1"/>
-      <c r="AD36" s="10"/>
-      <c r="AE36" s="7"/>
-      <c r="AF36" s="10"/>
-      <c r="AG36" s="10"/>
+      <c r="AD36" s="8"/>
+      <c r="AE36" s="5"/>
+      <c r="AF36" s="8"/>
+      <c r="AG36" s="8"/>
       <c r="AH36" s="2"/>
       <c r="AI36" s="2"/>
       <c r="AJ36" s="2"/>
-      <c r="AK36" s="10"/>
-      <c r="AL36" s="10"/>
+      <c r="AK36" s="8"/>
+      <c r="AL36" s="8"/>
       <c r="AM36" s="2"/>
       <c r="AN36" s="2"/>
       <c r="AO36" s="2"/>
       <c r="AP36" s="2"/>
     </row>
     <row r="37" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="58" t="s">
+      <c r="C37" s="25" t="s">
         <v>10</v>
       </c>
       <c r="D37" s="2"/>
@@ -2599,46 +2579,46 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="7"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="5"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="7"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="5"/>
       <c r="R37" s="2"/>
-      <c r="S37" s="10"/>
+      <c r="S37" s="8"/>
       <c r="T37" s="2"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-      <c r="W37" s="29"/>
-      <c r="X37" s="7"/>
+      <c r="U37" s="20"/>
+      <c r="V37" s="20"/>
+      <c r="W37" s="20"/>
+      <c r="X37" s="5"/>
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="2"/>
       <c r="AD37" s="1"/>
-      <c r="AE37" s="7"/>
-      <c r="AF37" s="10"/>
-      <c r="AG37" s="10"/>
+      <c r="AE37" s="5"/>
+      <c r="AF37" s="8"/>
+      <c r="AG37" s="8"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
       <c r="AJ37" s="2"/>
-      <c r="AK37" s="10"/>
-      <c r="AL37" s="10"/>
+      <c r="AK37" s="8"/>
+      <c r="AL37" s="8"/>
       <c r="AM37" s="2"/>
       <c r="AN37" s="2"/>
       <c r="AO37" s="2"/>
       <c r="AP37" s="2"/>
     </row>
     <row r="38" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="59" t="s">
+      <c r="C38" s="26" t="s">
         <v>11</v>
       </c>
       <c r="D38" s="2"/>
@@ -2646,186 +2626,182 @@
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="7"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="5"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
-      <c r="P38" s="10"/>
-      <c r="Q38" s="7"/>
+      <c r="P38" s="8"/>
+      <c r="Q38" s="5"/>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="2"/>
       <c r="V38" s="2"/>
-      <c r="W38" s="10"/>
-      <c r="X38" s="7"/>
-      <c r="Y38" s="29"/>
-      <c r="Z38" s="29"/>
-      <c r="AA38" s="29"/>
-      <c r="AB38" s="29"/>
-      <c r="AC38" s="29"/>
-      <c r="AD38" s="10"/>
-      <c r="AE38" s="7"/>
+      <c r="W38" s="8"/>
+      <c r="X38" s="5"/>
+      <c r="Y38" s="20"/>
+      <c r="Z38" s="20"/>
+      <c r="AA38" s="20"/>
+      <c r="AB38" s="20"/>
+      <c r="AC38" s="20"/>
+      <c r="AD38" s="8"/>
+      <c r="AE38" s="5"/>
       <c r="AF38" s="2"/>
       <c r="AG38" s="2"/>
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="1"/>
-      <c r="AL38" s="10"/>
+      <c r="AL38" s="8"/>
       <c r="AM38" s="2"/>
       <c r="AN38" s="2"/>
       <c r="AO38" s="2"/>
       <c r="AP38" s="2"/>
     </row>
     <row r="39" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B39" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="39"/>
+      <c r="B39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" s="26"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="10"/>
-      <c r="G39" s="10"/>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="10"/>
-      <c r="M39" s="10"/>
-      <c r="N39" s="10"/>
-      <c r="O39" s="10"/>
-      <c r="P39" s="10"/>
-      <c r="Q39" s="7"/>
-      <c r="R39" s="10"/>
-      <c r="S39" s="10"/>
-      <c r="T39" s="10"/>
-      <c r="U39" s="10"/>
-      <c r="V39" s="10"/>
-      <c r="W39" s="10"/>
-      <c r="X39" s="7"/>
-      <c r="Y39" s="10"/>
-      <c r="Z39" s="10"/>
-      <c r="AA39" s="10"/>
-      <c r="AB39" s="10"/>
-      <c r="AC39" s="10"/>
-      <c r="AD39" s="16"/>
-      <c r="AE39" s="16"/>
-      <c r="AF39" s="16"/>
-      <c r="AG39" s="16"/>
-      <c r="AH39" s="18"/>
-      <c r="AI39" s="18"/>
-      <c r="AJ39" s="18"/>
-      <c r="AK39" s="13"/>
-      <c r="AL39" s="10"/>
-      <c r="AM39" s="10"/>
-      <c r="AN39" s="10"/>
-      <c r="AO39" s="10"/>
-      <c r="AP39" s="10"/>
-      <c r="AQ39" s="11"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
+      <c r="O39" s="2"/>
+      <c r="P39" s="8"/>
+      <c r="Q39" s="5"/>
+      <c r="R39" s="2"/>
+      <c r="S39" s="2"/>
+      <c r="T39" s="2"/>
+      <c r="U39" s="2"/>
+      <c r="V39" s="2"/>
+      <c r="W39" s="8"/>
+      <c r="X39" s="5"/>
+      <c r="Y39" s="20"/>
+      <c r="Z39" s="20"/>
+      <c r="AA39" s="20"/>
+      <c r="AB39" s="20"/>
+      <c r="AC39" s="20"/>
+      <c r="AD39" s="8"/>
+      <c r="AE39" s="5"/>
+      <c r="AF39" s="2"/>
+      <c r="AG39" s="2"/>
+      <c r="AH39" s="1"/>
+      <c r="AI39" s="1"/>
+      <c r="AJ39" s="1"/>
+      <c r="AK39" s="1"/>
+      <c r="AL39" s="8"/>
+      <c r="AM39" s="2"/>
+      <c r="AN39" s="2"/>
+      <c r="AO39" s="2"/>
+      <c r="AP39" s="2"/>
     </row>
     <row r="40" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B40" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="59" t="s">
-        <v>11</v>
-      </c>
+      <c r="B40" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C40" s="26"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="10"/>
-      <c r="J40" s="7"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="5"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="2"/>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-      <c r="P40" s="10"/>
-      <c r="Q40" s="7"/>
+      <c r="P40" s="8"/>
+      <c r="Q40" s="5"/>
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="2"/>
       <c r="V40" s="2"/>
-      <c r="W40" s="10"/>
-      <c r="X40" s="7"/>
-      <c r="Y40" s="2"/>
-      <c r="Z40" s="2"/>
-      <c r="AA40" s="2"/>
-      <c r="AB40" s="2"/>
-      <c r="AC40" s="2"/>
-      <c r="AD40" s="29"/>
+      <c r="W40" s="8"/>
+      <c r="X40" s="5"/>
+      <c r="Y40" s="20"/>
+      <c r="Z40" s="20"/>
+      <c r="AA40" s="20"/>
+      <c r="AB40" s="20"/>
+      <c r="AC40" s="20"/>
+      <c r="AD40" s="8"/>
       <c r="AE40" s="5"/>
-      <c r="AF40" s="29"/>
-      <c r="AG40" s="29"/>
-      <c r="AH40" s="2"/>
-      <c r="AI40" s="2"/>
-      <c r="AJ40" s="2"/>
+      <c r="AF40" s="2"/>
+      <c r="AG40" s="2"/>
+      <c r="AH40" s="1"/>
+      <c r="AI40" s="1"/>
+      <c r="AJ40" s="1"/>
       <c r="AK40" s="1"/>
-      <c r="AL40" s="10"/>
-      <c r="AM40" s="10"/>
-      <c r="AN40" s="10"/>
-      <c r="AO40" s="10"/>
+      <c r="AL40" s="8"/>
+      <c r="AM40" s="2"/>
+      <c r="AN40" s="2"/>
+      <c r="AO40" s="2"/>
       <c r="AP40" s="2"/>
     </row>
     <row r="41" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B41" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="C41" s="60" t="s">
-        <v>10</v>
-      </c>
+      <c r="B41" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="28"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="10"/>
-      <c r="J41" s="7"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="10"/>
-      <c r="Q41" s="7"/>
-      <c r="R41" s="2"/>
-      <c r="S41" s="2"/>
-      <c r="T41" s="2"/>
-      <c r="U41" s="2"/>
-      <c r="V41" s="2"/>
-      <c r="W41" s="10"/>
-      <c r="X41" s="7"/>
-      <c r="Y41" s="2"/>
-      <c r="Z41" s="2"/>
-      <c r="AA41" s="2"/>
-      <c r="AB41" s="2"/>
-      <c r="AC41" s="2"/>
-      <c r="AD41" s="10"/>
-      <c r="AE41" s="7"/>
-      <c r="AF41" s="2"/>
-      <c r="AG41" s="1"/>
-      <c r="AH41" s="29"/>
-      <c r="AI41" s="29"/>
-      <c r="AJ41" s="2"/>
-      <c r="AK41" s="10"/>
-      <c r="AL41" s="10"/>
-      <c r="AM41" s="10"/>
-      <c r="AN41" s="10"/>
-      <c r="AO41" s="10"/>
-      <c r="AP41" s="2"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="5"/>
+      <c r="K41" s="8"/>
+      <c r="L41" s="8"/>
+      <c r="M41" s="8"/>
+      <c r="N41" s="8"/>
+      <c r="O41" s="8"/>
+      <c r="P41" s="8"/>
+      <c r="Q41" s="5"/>
+      <c r="R41" s="8"/>
+      <c r="S41" s="8"/>
+      <c r="T41" s="8"/>
+      <c r="U41" s="8"/>
+      <c r="V41" s="8"/>
+      <c r="W41" s="8"/>
+      <c r="X41" s="5"/>
+      <c r="Y41" s="8"/>
+      <c r="Z41" s="8"/>
+      <c r="AA41" s="8"/>
+      <c r="AB41" s="8"/>
+      <c r="AC41" s="8"/>
+      <c r="AD41" s="12"/>
+      <c r="AE41" s="12"/>
+      <c r="AF41" s="12"/>
+      <c r="AG41" s="12"/>
+      <c r="AH41" s="14"/>
+      <c r="AI41" s="14"/>
+      <c r="AJ41" s="14"/>
+      <c r="AK41" s="11"/>
+      <c r="AL41" s="8"/>
+      <c r="AM41" s="8"/>
+      <c r="AN41" s="8"/>
+      <c r="AO41" s="8"/>
+      <c r="AP41" s="8"/>
+      <c r="AQ41" s="9"/>
     </row>
     <row r="42" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B42" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" s="59" t="s">
+      <c r="B42" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="26" t="s">
         <v>11</v>
       </c>
       <c r="D42" s="2"/>
@@ -2833,290 +2809,362 @@
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
-      <c r="I42" s="10"/>
-      <c r="J42" s="7"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="5"/>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
       <c r="M42" s="2"/>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
-      <c r="P42" s="10"/>
-      <c r="Q42" s="7"/>
+      <c r="P42" s="8"/>
+      <c r="Q42" s="5"/>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="2"/>
       <c r="V42" s="2"/>
-      <c r="W42" s="10"/>
-      <c r="X42" s="7"/>
+      <c r="W42" s="8"/>
+      <c r="X42" s="5"/>
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
       <c r="AC42" s="2"/>
-      <c r="AD42" s="10"/>
-      <c r="AE42" s="7"/>
-      <c r="AF42" s="2"/>
-      <c r="AG42" s="2"/>
+      <c r="AD42" s="20"/>
+      <c r="AE42" s="4"/>
+      <c r="AF42" s="20"/>
+      <c r="AG42" s="20"/>
       <c r="AH42" s="2"/>
-      <c r="AI42" s="1"/>
-      <c r="AJ42" s="29"/>
+      <c r="AI42" s="2"/>
+      <c r="AJ42" s="2"/>
       <c r="AK42" s="1"/>
-      <c r="AL42" s="10"/>
-      <c r="AM42" s="10"/>
-      <c r="AN42" s="10"/>
-      <c r="AO42" s="12"/>
+      <c r="AL42" s="8"/>
+      <c r="AM42" s="8"/>
+      <c r="AN42" s="8"/>
+      <c r="AO42" s="8"/>
       <c r="AP42" s="2"/>
     </row>
     <row r="43" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="20"/>
-      <c r="R43" s="20"/>
-      <c r="S43" s="20"/>
-      <c r="T43" s="20"/>
-      <c r="U43" s="20"/>
-      <c r="V43" s="20"/>
-      <c r="W43" s="20"/>
-      <c r="X43" s="20"/>
-      <c r="Y43" s="20"/>
-      <c r="Z43" s="20"/>
-      <c r="AA43" s="20"/>
-      <c r="AB43" s="20"/>
-      <c r="AC43" s="20"/>
-      <c r="AD43" s="20"/>
-      <c r="AE43" s="20"/>
-      <c r="AF43" s="20"/>
-      <c r="AG43" s="20"/>
+      <c r="B43" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="5"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="8"/>
+      <c r="Q43" s="5"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="8"/>
+      <c r="X43" s="5"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="2"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="8"/>
+      <c r="AE43" s="5"/>
+      <c r="AF43" s="2"/>
+      <c r="AG43" s="1"/>
       <c r="AH43" s="20"/>
       <c r="AI43" s="20"/>
-      <c r="AJ43" s="20"/>
-      <c r="AK43" s="20"/>
-      <c r="AL43" s="20"/>
-      <c r="AM43" s="20"/>
-      <c r="AN43" s="20"/>
-      <c r="AO43" s="20"/>
-      <c r="AP43" s="20"/>
+      <c r="AJ43" s="2"/>
+      <c r="AK43" s="8"/>
+      <c r="AL43" s="8"/>
+      <c r="AM43" s="8"/>
+      <c r="AN43" s="8"/>
+      <c r="AO43" s="8"/>
+      <c r="AP43" s="2"/>
     </row>
     <row r="44" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
-      <c r="M44" s="20"/>
-      <c r="N44" s="20"/>
-      <c r="O44" s="20"/>
-      <c r="P44" s="20"/>
-      <c r="Q44" s="20"/>
-      <c r="R44" s="20"/>
-      <c r="S44" s="20"/>
-      <c r="T44" s="20"/>
-      <c r="U44" s="20"/>
-      <c r="V44" s="20"/>
-      <c r="W44" s="20"/>
-      <c r="X44" s="20"/>
-      <c r="Y44" s="20"/>
-      <c r="Z44" s="20"/>
-      <c r="AA44" s="20"/>
-      <c r="AB44" s="20"/>
-      <c r="AC44" s="20"/>
-      <c r="AD44" s="20"/>
-      <c r="AE44" s="20"/>
-      <c r="AF44" s="20"/>
-      <c r="AG44" s="20"/>
+      <c r="B44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C44" s="42"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="8"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="2"/>
+      <c r="S44" s="2"/>
+      <c r="T44" s="2"/>
+      <c r="U44" s="2"/>
+      <c r="V44" s="2"/>
+      <c r="W44" s="8"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="2"/>
+      <c r="Z44" s="2"/>
+      <c r="AA44" s="2"/>
+      <c r="AB44" s="2"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="8"/>
+      <c r="AE44" s="5"/>
+      <c r="AF44" s="2"/>
+      <c r="AG44" s="1"/>
       <c r="AH44" s="20"/>
       <c r="AI44" s="20"/>
-      <c r="AJ44" s="20"/>
-      <c r="AK44" s="20"/>
-      <c r="AL44" s="20"/>
-      <c r="AM44" s="20"/>
-      <c r="AN44" s="20"/>
-      <c r="AO44" s="20"/>
-      <c r="AP44" s="20"/>
+      <c r="AJ44" s="2"/>
+      <c r="AK44" s="8"/>
+      <c r="AL44" s="8"/>
+      <c r="AM44" s="8"/>
+      <c r="AN44" s="8"/>
+      <c r="AO44" s="8"/>
+      <c r="AP44" s="2"/>
     </row>
     <row r="45" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
-      <c r="K45" s="20"/>
-      <c r="L45" s="20"/>
-      <c r="M45" s="20"/>
-      <c r="N45" s="20"/>
-      <c r="O45" s="20"/>
-      <c r="P45" s="20"/>
-      <c r="Q45" s="20"/>
-      <c r="R45" s="20"/>
-      <c r="S45" s="20"/>
-      <c r="T45" s="20"/>
-      <c r="U45" s="20"/>
-      <c r="V45" s="20"/>
-      <c r="W45" s="20"/>
-      <c r="X45" s="20"/>
-      <c r="Y45" s="20"/>
-      <c r="Z45" s="20"/>
-      <c r="AA45" s="20"/>
-      <c r="AB45" s="20"/>
-      <c r="AC45" s="20"/>
-      <c r="AD45" s="20"/>
-      <c r="AE45" s="20"/>
-      <c r="AF45" s="20"/>
-      <c r="AG45" s="20"/>
+      <c r="B45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C45" s="43"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+      <c r="H45" s="2"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="2"/>
+      <c r="N45" s="2"/>
+      <c r="O45" s="2"/>
+      <c r="P45" s="8"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="2"/>
+      <c r="S45" s="2"/>
+      <c r="T45" s="2"/>
+      <c r="U45" s="2"/>
+      <c r="V45" s="2"/>
+      <c r="W45" s="8"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="2"/>
+      <c r="Z45" s="2"/>
+      <c r="AA45" s="2"/>
+      <c r="AB45" s="2"/>
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="8"/>
+      <c r="AE45" s="5"/>
+      <c r="AF45" s="2"/>
+      <c r="AG45" s="1"/>
       <c r="AH45" s="20"/>
       <c r="AI45" s="20"/>
-      <c r="AJ45" s="20"/>
-      <c r="AK45" s="20"/>
-      <c r="AL45" s="20"/>
-      <c r="AM45" s="20"/>
-      <c r="AN45" s="20"/>
-      <c r="AO45" s="20"/>
-      <c r="AP45" s="20"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B57" s="24"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="34"/>
-      <c r="B58" s="24"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="34"/>
-      <c r="B59" s="24"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="25"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="26"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B62" s="25"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B63" s="26"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="s">
+      <c r="AJ45" s="2"/>
+      <c r="AK45" s="8"/>
+      <c r="AL45" s="8"/>
+      <c r="AM45" s="8"/>
+      <c r="AN45" s="8"/>
+      <c r="AO45" s="8"/>
+      <c r="AP45" s="2"/>
+    </row>
+    <row r="46" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="B46" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B64" s="27"/>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" s="26"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B66" s="27"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B67" s="26"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="25"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B69" s="27"/>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B70" s="26"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B71" s="25"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B72" s="27"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B73" s="27"/>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B74" s="25"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B75" s="27"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="28"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="28"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="28"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="8"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="2"/>
+      <c r="S46" s="2"/>
+      <c r="T46" s="2"/>
+      <c r="U46" s="2"/>
+      <c r="V46" s="2"/>
+      <c r="W46" s="8"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="2"/>
+      <c r="Z46" s="2"/>
+      <c r="AA46" s="2"/>
+      <c r="AB46" s="2"/>
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="8"/>
+      <c r="AE46" s="5"/>
+      <c r="AF46" s="2"/>
+      <c r="AG46" s="2"/>
+      <c r="AH46" s="2"/>
+      <c r="AI46" s="1"/>
+      <c r="AJ46" s="20"/>
+      <c r="AK46" s="1"/>
+      <c r="AL46" s="8"/>
+      <c r="AM46" s="8"/>
+      <c r="AN46" s="8"/>
+      <c r="AO46" s="10"/>
+      <c r="AP46" s="2"/>
+    </row>
+    <row r="47" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
+      <c r="T47" s="16"/>
+      <c r="U47" s="16"/>
+      <c r="V47" s="16"/>
+      <c r="W47" s="16"/>
+      <c r="X47" s="16"/>
+      <c r="Y47" s="16"/>
+      <c r="Z47" s="16"/>
+      <c r="AA47" s="16"/>
+      <c r="AB47" s="16"/>
+      <c r="AC47" s="16"/>
+      <c r="AD47" s="16"/>
+      <c r="AE47" s="16"/>
+      <c r="AF47" s="16"/>
+      <c r="AG47" s="16"/>
+      <c r="AH47" s="16"/>
+      <c r="AI47" s="16"/>
+      <c r="AJ47" s="16"/>
+      <c r="AK47" s="16"/>
+      <c r="AL47" s="16"/>
+      <c r="AM47" s="16"/>
+      <c r="AN47" s="16"/>
+      <c r="AO47" s="16"/>
+      <c r="AP47" s="16"/>
+    </row>
+    <row r="48" spans="2:43" x14ac:dyDescent="0.25">
+      <c r="C48" s="16"/>
+      <c r="D48" s="16"/>
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="16"/>
+      <c r="I48" s="16"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
+      <c r="M48" s="16"/>
+      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
+      <c r="P48" s="16"/>
+      <c r="Q48" s="16"/>
+      <c r="R48" s="16"/>
+      <c r="S48" s="16"/>
+      <c r="T48" s="16"/>
+      <c r="U48" s="16"/>
+      <c r="V48" s="16"/>
+      <c r="W48" s="16"/>
+      <c r="X48" s="16"/>
+      <c r="Y48" s="16"/>
+      <c r="Z48" s="16"/>
+      <c r="AA48" s="16"/>
+      <c r="AB48" s="16"/>
+      <c r="AC48" s="16"/>
+      <c r="AD48" s="16"/>
+      <c r="AE48" s="16"/>
+      <c r="AF48" s="16"/>
+      <c r="AG48" s="16"/>
+      <c r="AH48" s="16"/>
+      <c r="AI48" s="16"/>
+      <c r="AJ48" s="16"/>
+      <c r="AK48" s="16"/>
+      <c r="AL48" s="16"/>
+      <c r="AM48" s="16"/>
+      <c r="AN48" s="16"/>
+      <c r="AO48" s="16"/>
+      <c r="AP48" s="16"/>
+    </row>
+    <row r="49" spans="3:42" x14ac:dyDescent="0.25">
+      <c r="C49" s="16"/>
+      <c r="D49" s="16"/>
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="16"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16"/>
+      <c r="M49" s="16"/>
+      <c r="N49" s="16"/>
+      <c r="O49" s="16"/>
+      <c r="P49" s="16"/>
+      <c r="Q49" s="16"/>
+      <c r="R49" s="16"/>
+      <c r="S49" s="16"/>
+      <c r="T49" s="16"/>
+      <c r="U49" s="16"/>
+      <c r="V49" s="16"/>
+      <c r="W49" s="16"/>
+      <c r="X49" s="16"/>
+      <c r="Y49" s="16"/>
+      <c r="Z49" s="16"/>
+      <c r="AA49" s="16"/>
+      <c r="AB49" s="16"/>
+      <c r="AC49" s="16"/>
+      <c r="AD49" s="16"/>
+      <c r="AE49" s="16"/>
+      <c r="AF49" s="16"/>
+      <c r="AG49" s="16"/>
+      <c r="AH49" s="16"/>
+      <c r="AI49" s="16"/>
+      <c r="AJ49" s="16"/>
+      <c r="AK49" s="16"/>
+      <c r="AL49" s="16"/>
+      <c r="AM49" s="16"/>
+      <c r="AN49" s="16"/>
+      <c r="AO49" s="16"/>
+      <c r="AP49" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C12:C16"/>
+    <mergeCell ref="C43:C45"/>
+    <mergeCell ref="C34:C35"/>
     <mergeCell ref="C27:C31"/>
     <mergeCell ref="C32:C33"/>
-    <mergeCell ref="C34:C35"/>
     <mergeCell ref="A2:AP2"/>
-    <mergeCell ref="A57:A59"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="M4:AP4"/>
     <mergeCell ref="D4:L4"/>
@@ -3124,10 +3172,6 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C12:C16"/>
     <mergeCell ref="C20:C22"/>
     <mergeCell ref="C17:C19"/>
     <mergeCell ref="C23:C25"/>

</xml_diff>